<commit_message>
GameData bugfix, ConcertController bugfix
</commit_message>
<xml_diff>
--- a/TapBand_SRC/Assets/Data/GameData.xlsx
+++ b/TapBand_SRC/Assets/Data/GameData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -79,6 +79,33 @@
   </si>
   <si>
     <t>Veresegyházi Falunap</t>
+  </si>
+  <si>
+    <t>Falunap 2</t>
+  </si>
+  <si>
+    <t>Falunap 3</t>
+  </si>
+  <si>
+    <t>Falunap 4</t>
+  </si>
+  <si>
+    <t>Falunap 5</t>
+  </si>
+  <si>
+    <t>Falunap 6</t>
+  </si>
+  <si>
+    <t>Falunap 7</t>
+  </si>
+  <si>
+    <t>Falunap 8</t>
+  </si>
+  <si>
+    <t>Falunap 9</t>
+  </si>
+  <si>
+    <t>Falunap 10</t>
   </si>
   <si>
     <t>Level</t>
@@ -568,6 +595,1326 @@
         <v>2.0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="F12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="F13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="F14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="F15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="F17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="F18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="F19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>55.0</v>
+      </c>
+      <c r="F20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="F22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="F23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="F24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="F25" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="F27" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="F28" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="F29" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>55.0</v>
+      </c>
+      <c r="F30" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3">
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="F32" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3">
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="F33" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="F34" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3">
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="F35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F36" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3">
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="F37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3">
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="F38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3">
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="F39" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3">
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>55.0</v>
+      </c>
+      <c r="F40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F41" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3">
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="F42" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3">
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="F43" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3">
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="F44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3">
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="F45" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F46" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="F47" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3">
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="F48" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3">
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="F49" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>55.0</v>
+      </c>
+      <c r="F50" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="D51" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F51" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+    </row>
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="F2:F1000">
@@ -652,6 +1999,132 @@
         <v>150.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>110.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>250.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3">
+        <v>130.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>300.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3">
+        <v>150.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>350.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3">
+        <v>170.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>400.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3">
+        <v>190.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>450.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3">
+        <v>210.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>500.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3">
+        <v>230.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>550.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3">
+        <v>250.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>600.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -672,19 +2145,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
@@ -1407,19 +2880,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
@@ -1447,13 +2920,13 @@
         <v>101.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E2" s="3">
         <v>100.0</v>
@@ -1467,13 +2940,13 @@
         <v>102.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3">
         <v>150.0</v>
@@ -1487,7 +2960,7 @@
         <v>103.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3">
         <v>3.0</v>
@@ -1525,7 +2998,7 @@
         <v>104.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3">
         <v>4.0</v>
@@ -1543,7 +3016,7 @@
         <v>105.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3">
         <v>5.0</v>
@@ -1561,7 +3034,7 @@
         <v>106.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3">
         <v>6.0</v>
@@ -1579,7 +3052,7 @@
         <v>107.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3">
         <v>7.0</v>
@@ -1597,7 +3070,7 @@
         <v>108.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3">
         <v>8.0</v>
@@ -1615,7 +3088,7 @@
         <v>109.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3">
         <v>9.0</v>
@@ -1633,7 +3106,7 @@
         <v>110.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3">
         <v>10.0</v>
@@ -1651,13 +3124,13 @@
         <v>201.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3">
         <v>1.0</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3">
         <v>80.0</v>
@@ -1671,13 +3144,13 @@
         <v>202.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3">
         <v>2.0</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E13" s="3">
         <v>120.0</v>
@@ -1691,7 +3164,7 @@
         <v>203.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3">
         <v>3.0</v>
@@ -1708,7 +3181,7 @@
         <v>204.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3">
         <v>4.0</v>
@@ -1725,7 +3198,7 @@
         <v>205.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3">
         <v>5.0</v>
@@ -1742,7 +3215,7 @@
         <v>206.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3">
         <v>6.0</v>
@@ -1759,7 +3232,7 @@
         <v>207.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3">
         <v>7.0</v>
@@ -1776,7 +3249,7 @@
         <v>208.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3">
         <v>8.0</v>
@@ -1793,7 +3266,7 @@
         <v>209.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3">
         <v>9.0</v>
@@ -1810,7 +3283,7 @@
         <v>210.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3">
         <v>10.0</v>
@@ -1828,13 +3301,13 @@
         <v>301.0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3">
         <v>1.0</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E22" s="3">
         <v>50.0</v>
@@ -1848,13 +3321,13 @@
         <v>302.0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3">
         <v>2.0</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E23" s="3">
         <v>90.0</v>
@@ -1868,7 +3341,7 @@
         <v>303.0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C24" s="3">
         <v>3.0</v>
@@ -1885,7 +3358,7 @@
         <v>304.0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3">
         <v>4.0</v>
@@ -1902,7 +3375,7 @@
         <v>305.0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3">
         <v>5.0</v>
@@ -1919,7 +3392,7 @@
         <v>306.0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C27" s="3">
         <v>6.0</v>
@@ -1936,7 +3409,7 @@
         <v>307.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C28" s="3">
         <v>7.0</v>
@@ -1953,7 +3426,7 @@
         <v>308.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C29" s="3">
         <v>8.0</v>
@@ -1970,7 +3443,7 @@
         <v>309.0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C30" s="3">
         <v>9.0</v>
@@ -1987,7 +3460,7 @@
         <v>310.0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C31" s="3">
         <v>10.0</v>
@@ -2004,13 +3477,13 @@
         <v>401.0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3">
         <v>1.0</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E32" s="3">
         <v>150.0</v>
@@ -2024,13 +3497,13 @@
         <v>402.0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C33" s="3">
         <v>2.0</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E33" s="3">
         <v>200.0</v>
@@ -2044,7 +3517,7 @@
         <v>403.0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C34" s="3">
         <v>3.0</v>
@@ -2061,7 +3534,7 @@
         <v>404.0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C35" s="3">
         <v>4.0</v>
@@ -2078,7 +3551,7 @@
         <v>405.0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C36" s="3">
         <v>5.0</v>
@@ -2095,7 +3568,7 @@
         <v>406.0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C37" s="3">
         <v>6.0</v>
@@ -2112,7 +3585,7 @@
         <v>407.0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C38" s="3">
         <v>7.0</v>
@@ -2129,7 +3602,7 @@
         <v>408.0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C39" s="3">
         <v>8.0</v>
@@ -2146,7 +3619,7 @@
         <v>409.0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C40" s="3">
         <v>9.0</v>
@@ -2163,7 +3636,7 @@
         <v>410.0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C41" s="3">
         <v>10.0</v>
@@ -2203,22 +3676,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -2246,16 +3719,16 @@
         <v>101.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="F2" s="3">
         <v>0.0</v>
@@ -2269,13 +3742,13 @@
         <v>102.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E3" s="3">
         <v>75.0</v>
@@ -2292,13 +3765,13 @@
         <v>103.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3">
         <v>3.0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E4" s="3">
         <v>100.0</v>
@@ -2315,16 +3788,16 @@
         <v>201.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3">
         <v>1.0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="F5" s="3">
         <v>1.0</v>
@@ -2338,13 +3811,13 @@
         <v>202.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3">
         <v>2.0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3">
         <v>75.0</v>
@@ -2361,13 +3834,13 @@
         <v>203.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3">
         <v>3.0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E7" s="3">
         <v>100.0</v>
@@ -2407,7 +3880,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2438,7 +3911,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3">
         <v>1524.0</v>
@@ -2449,7 +3922,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C3" s="3">
         <v>2048.0</v>
@@ -2460,7 +3933,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
New Gamedata for Test
Yeeeeeee
</commit_message>
<xml_diff>
--- a/TapBand_SRC/Assets/Data/GameData.xlsx
+++ b/TapBand_SRC/Assets/Data/GameData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -75,10 +75,7 @@
     <t>FanReward</t>
   </si>
   <si>
-    <t>Kazincbarcikai Szabadidős Napok</t>
-  </si>
-  <si>
-    <t>Veresegyházi Falunap</t>
+    <t>Falunap 1</t>
   </si>
   <si>
     <t>Falunap 2</t>
@@ -132,37 +129,133 @@
     <t>KEYBOARD</t>
   </si>
   <si>
-    <t>Unholy Mageblade</t>
-  </si>
-  <si>
-    <t>Warped Silver Defender</t>
+    <t>Kinslayer</t>
+  </si>
+  <si>
+    <t>Blazeguard</t>
+  </si>
+  <si>
+    <t>Striker</t>
+  </si>
+  <si>
+    <t>Jade Infused Quickblade</t>
+  </si>
+  <si>
+    <t>Skyfall Doomblade</t>
+  </si>
+  <si>
+    <t>Flaming Copper Spellblade</t>
+  </si>
+  <si>
+    <t>Isolated Glass Broadsword</t>
+  </si>
+  <si>
+    <t>Extinction, Slicer of Trials</t>
+  </si>
+  <si>
+    <t>Hell's Scream, Sword of the Wretched</t>
+  </si>
+  <si>
+    <t>Nightcrackle, Savagery of the King</t>
   </si>
   <si>
     <t>BASS</t>
   </si>
   <si>
-    <t>Brutality, Conqueror of Perdition</t>
-  </si>
-  <si>
-    <t>Ragnarok, Sculptor of Wasted Time</t>
+    <t>Grasscutter</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>Orenmir</t>
+  </si>
+  <si>
+    <t>Vicious Blade</t>
+  </si>
+  <si>
+    <t>Ancient Blade</t>
+  </si>
+  <si>
+    <t>Howling Glass Quickblade</t>
+  </si>
+  <si>
+    <t>Ebon Glass Protector</t>
+  </si>
+  <si>
+    <t>Shadow Strike, Dawn of Blessed Fortune</t>
+  </si>
+  <si>
+    <t>Faithkeeper, Foe of the Champion</t>
+  </si>
+  <si>
+    <t>Misery, Terror of the Whispers</t>
   </si>
   <si>
     <t>GUITAR</t>
   </si>
   <si>
-    <t>Honor's Call</t>
-  </si>
-  <si>
-    <t>Hatred's Bite, Gift of the Cataclysm</t>
+    <t>Lazarus</t>
+  </si>
+  <si>
+    <t>Devine</t>
+  </si>
+  <si>
+    <t>Widow Maker</t>
+  </si>
+  <si>
+    <t>Mourning Etcher</t>
+  </si>
+  <si>
+    <t>Singing Claymore</t>
+  </si>
+  <si>
+    <t>Massive Glass Sculptor</t>
+  </si>
+  <si>
+    <t>Tyrannical Skeletal Reaver</t>
+  </si>
+  <si>
+    <t>The Black Blade, Bringer of Shadows</t>
+  </si>
+  <si>
+    <t>Hope's End, Tribute of Phantoms</t>
+  </si>
+  <si>
+    <t>Spike, Ender of Subtlety</t>
   </si>
   <si>
     <t>DRUM</t>
   </si>
   <si>
-    <t>Frenzy, Ender of the Serpent</t>
-  </si>
-  <si>
-    <t>Chaos, Shortsword of Eternal Sorrow</t>
+    <t>Blazefury</t>
+  </si>
+  <si>
+    <t>Mercy</t>
+  </si>
+  <si>
+    <t>Worldslayer</t>
+  </si>
+  <si>
+    <t>Wretched Katana</t>
+  </si>
+  <si>
+    <t>Howling Razor</t>
+  </si>
+  <si>
+    <t>Dragon's Gold Greatsword</t>
+  </si>
+  <si>
+    <t>Soulcursed Diamond Spellblade</t>
+  </si>
+  <si>
+    <t>Hellreaver, Savagery of Inception</t>
+  </si>
+  <si>
+    <t>Justifier, Crusader of Immortality</t>
+  </si>
+  <si>
+    <t>Reign, Warblade of Illumination</t>
   </si>
   <si>
     <t>MerchType</t>
@@ -177,25 +270,25 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Booth</t>
-  </si>
-  <si>
-    <t>Shop</t>
+    <t>Hellfire</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Dawnbreaker</t>
   </si>
   <si>
     <t>QUALITY</t>
   </si>
   <si>
-    <t>Stickers</t>
-  </si>
-  <si>
-    <t>T-Shirts</t>
-  </si>
-  <si>
-    <t>Signed Guitars</t>
+    <t>Renovated Skewer</t>
+  </si>
+  <si>
+    <t>Bloodlord's Rapier</t>
+  </si>
+  <si>
+    <t>Sorrow's Diamond Deflector</t>
   </si>
   <si>
     <t>Value</t>
@@ -225,12 +318,12 @@
       <sz val="10.0"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="'�Palatino Linotype�'"/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -269,18 +362,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2111,20 +2202,6 @@
         <v>550.0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="3">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="3">
-        <v>250.0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>600.0</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2145,19 +2222,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
@@ -2188,16 +2265,16 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="3">
-        <v>1.1</v>
+        <v>1.0</v>
       </c>
       <c r="D2" s="3">
-        <v>1.15</v>
+        <v>1.0</v>
       </c>
       <c r="E2" s="3">
-        <v>1.5</v>
+        <v>1.0</v>
       </c>
       <c r="F2" s="3">
-        <v>10000.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="3">
@@ -2217,7 +2294,7 @@
         <v>1.6</v>
       </c>
       <c r="F3" s="3">
-        <v>10000.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="4">
@@ -2237,7 +2314,7 @@
         <v>1.7</v>
       </c>
       <c r="F4" s="3">
-        <v>10000.0</v>
+        <v>140.0</v>
       </c>
     </row>
     <row r="5">
@@ -2257,7 +2334,7 @@
         <v>1.8</v>
       </c>
       <c r="F5" s="3">
-        <v>10000.0</v>
+        <v>160.0</v>
       </c>
     </row>
     <row r="6">
@@ -2277,7 +2354,7 @@
         <v>1.9</v>
       </c>
       <c r="F6" s="3">
-        <v>10000.0</v>
+        <v>180.0</v>
       </c>
     </row>
     <row r="7">
@@ -2297,7 +2374,7 @@
         <v>2.0</v>
       </c>
       <c r="F7" s="3">
-        <v>10000.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="8">
@@ -2317,7 +2394,7 @@
         <v>2.1</v>
       </c>
       <c r="F8" s="3">
-        <v>10000.0</v>
+        <v>220.0</v>
       </c>
     </row>
     <row r="9">
@@ -2337,7 +2414,7 @@
         <v>2.2</v>
       </c>
       <c r="F9" s="3">
-        <v>10000.0</v>
+        <v>240.0</v>
       </c>
     </row>
     <row r="10">
@@ -2357,7 +2434,7 @@
         <v>2.3</v>
       </c>
       <c r="F10" s="3">
-        <v>10000.0</v>
+        <v>260.0</v>
       </c>
     </row>
     <row r="11">
@@ -2377,7 +2454,7 @@
         <v>2.4</v>
       </c>
       <c r="F11" s="3">
-        <v>10000.0</v>
+        <v>280.0</v>
       </c>
     </row>
     <row r="12">
@@ -2397,7 +2474,7 @@
         <v>2.5</v>
       </c>
       <c r="F12" s="3">
-        <v>10000.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="13">
@@ -2417,7 +2494,7 @@
         <v>2.6</v>
       </c>
       <c r="F13" s="3">
-        <v>10000.0</v>
+        <v>320.0</v>
       </c>
     </row>
     <row r="14">
@@ -2437,7 +2514,7 @@
         <v>2.7</v>
       </c>
       <c r="F14" s="3">
-        <v>10000.0</v>
+        <v>340.0</v>
       </c>
     </row>
     <row r="15">
@@ -2457,7 +2534,7 @@
         <v>2.8</v>
       </c>
       <c r="F15" s="3">
-        <v>10000.0</v>
+        <v>360.0</v>
       </c>
     </row>
     <row r="16">
@@ -2477,7 +2554,7 @@
         <v>2.90000000000001</v>
       </c>
       <c r="F16" s="3">
-        <v>10000.0</v>
+        <v>380.0</v>
       </c>
     </row>
     <row r="17">
@@ -2497,7 +2574,7 @@
         <v>3.00000000000001</v>
       </c>
       <c r="F17" s="3">
-        <v>10000.0</v>
+        <v>400.0</v>
       </c>
     </row>
     <row r="18">
@@ -2517,7 +2594,7 @@
         <v>3.10000000000001</v>
       </c>
       <c r="F18" s="3">
-        <v>10000.0</v>
+        <v>420.0</v>
       </c>
     </row>
     <row r="19">
@@ -2537,7 +2614,7 @@
         <v>3.20000000000001</v>
       </c>
       <c r="F19" s="3">
-        <v>10000.0</v>
+        <v>440.0</v>
       </c>
     </row>
     <row r="20">
@@ -2557,7 +2634,7 @@
         <v>3.30000000000001</v>
       </c>
       <c r="F20" s="3">
-        <v>10000.0</v>
+        <v>460.0</v>
       </c>
     </row>
     <row r="21">
@@ -2577,7 +2654,7 @@
         <v>3.40000000000001</v>
       </c>
       <c r="F21" s="3">
-        <v>10000.0</v>
+        <v>480.0</v>
       </c>
     </row>
     <row r="22">
@@ -2597,7 +2674,7 @@
         <v>3.50000000000001</v>
       </c>
       <c r="F22" s="3">
-        <v>10000.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="23">
@@ -2617,7 +2694,7 @@
         <v>3.60000000000001</v>
       </c>
       <c r="F23" s="3">
-        <v>10000.0</v>
+        <v>520.0</v>
       </c>
     </row>
     <row r="24">
@@ -2637,7 +2714,7 @@
         <v>3.70000000000001</v>
       </c>
       <c r="F24" s="3">
-        <v>10000.0</v>
+        <v>540.0</v>
       </c>
     </row>
     <row r="25">
@@ -2657,7 +2734,7 @@
         <v>3.80000000000002</v>
       </c>
       <c r="F25" s="3">
-        <v>10000.0</v>
+        <v>560.0</v>
       </c>
     </row>
     <row r="26">
@@ -2677,7 +2754,7 @@
         <v>3.90000000000002</v>
       </c>
       <c r="F26" s="3">
-        <v>10000.0</v>
+        <v>580.0</v>
       </c>
     </row>
     <row r="27">
@@ -2697,7 +2774,7 @@
         <v>4.00000000000002</v>
       </c>
       <c r="F27" s="3">
-        <v>10000.0</v>
+        <v>600.0</v>
       </c>
     </row>
     <row r="28">
@@ -2717,7 +2794,7 @@
         <v>4.10000000000002</v>
       </c>
       <c r="F28" s="3">
-        <v>10000.0</v>
+        <v>620.0</v>
       </c>
     </row>
     <row r="29">
@@ -2737,7 +2814,7 @@
         <v>4.20000000000002</v>
       </c>
       <c r="F29" s="3">
-        <v>10000.0</v>
+        <v>640.0</v>
       </c>
     </row>
     <row r="30">
@@ -2757,7 +2834,7 @@
         <v>4.30000000000002</v>
       </c>
       <c r="F30" s="3">
-        <v>10000.0</v>
+        <v>660.0</v>
       </c>
     </row>
     <row r="31">
@@ -2777,7 +2854,7 @@
         <v>4.40000000000002</v>
       </c>
       <c r="F31" s="3">
-        <v>10000.0</v>
+        <v>680.0</v>
       </c>
     </row>
     <row r="32">
@@ -2797,7 +2874,7 @@
         <v>4.50000000000002</v>
       </c>
       <c r="F32" s="3">
-        <v>10000.0</v>
+        <v>700.0</v>
       </c>
     </row>
     <row r="33">
@@ -2817,7 +2894,7 @@
         <v>4.60000000000002</v>
       </c>
       <c r="F33" s="3">
-        <v>10000.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="34">
@@ -2837,7 +2914,7 @@
         <v>4.70000000000002</v>
       </c>
       <c r="F34" s="3">
-        <v>10000.0</v>
+        <v>740.0</v>
       </c>
     </row>
     <row r="35">
@@ -2857,7 +2934,7 @@
         <v>4.80000000000003</v>
       </c>
       <c r="F35" s="3">
-        <v>10000.0</v>
+        <v>760.0</v>
       </c>
     </row>
   </sheetData>
@@ -2872,7 +2949,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="33.43"/>
+    <col customWidth="1" min="4" max="4" width="38.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2880,19 +2957,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
@@ -2920,16 +2997,16 @@
         <v>101.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
+      <c r="D2" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="E2" s="3">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
       <c r="F2" s="3">
         <v>1.2</v>
@@ -2940,16 +3017,16 @@
         <v>102.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E3" s="3">
-        <v>150.0</v>
+        <v>7.0</v>
       </c>
       <c r="F3" s="3">
         <v>1.5</v>
@@ -2960,14 +3037,16 @@
         <v>103.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3">
         <v>3.0</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="E4" s="3">
-        <v>200.0</v>
+        <v>9.0</v>
       </c>
       <c r="F4" s="3">
         <v>1.8</v>
@@ -2998,14 +3077,16 @@
         <v>104.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="3">
         <v>4.0</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="E5" s="3">
-        <v>250.0</v>
+        <v>11.0</v>
       </c>
       <c r="F5" s="3">
         <v>2.1</v>
@@ -3016,14 +3097,16 @@
         <v>105.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
         <v>5.0</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="E6" s="3">
-        <v>300.0</v>
+        <v>13.0</v>
       </c>
       <c r="F6" s="3">
         <v>2.4</v>
@@ -3034,14 +3117,16 @@
         <v>106.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="3">
         <v>6.0</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="E7" s="3">
-        <v>350.0</v>
+        <v>15.0</v>
       </c>
       <c r="F7" s="3">
         <v>2.7</v>
@@ -3052,14 +3137,16 @@
         <v>107.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3">
         <v>7.0</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="E8" s="3">
-        <v>400.0</v>
+        <v>17.0</v>
       </c>
       <c r="F8" s="3">
         <v>3.0</v>
@@ -3070,14 +3157,16 @@
         <v>108.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3">
         <v>8.0</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="E9" s="3">
-        <v>450.0</v>
+        <v>19.0</v>
       </c>
       <c r="F9" s="3">
         <v>3.3</v>
@@ -3088,14 +3177,16 @@
         <v>109.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3">
         <v>9.0</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E10" s="3">
-        <v>500.0</v>
+        <v>21.0</v>
       </c>
       <c r="F10" s="3">
         <v>3.6</v>
@@ -3106,14 +3197,16 @@
         <v>110.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3">
         <v>10.0</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="E11" s="3">
-        <v>550.0</v>
+        <v>23.0</v>
       </c>
       <c r="F11" s="3">
         <v>3.9</v>
@@ -3124,19 +3217,19 @@
         <v>201.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3">
         <v>1.0</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>41</v>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="E12" s="3">
-        <v>80.0</v>
+        <v>5.0</v>
       </c>
       <c r="F12" s="3">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="13">
@@ -3144,19 +3237,19 @@
         <v>202.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C13" s="3">
         <v>2.0</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>42</v>
+      <c r="D13" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="E13" s="3">
-        <v>120.0</v>
+        <v>7.0</v>
       </c>
       <c r="F13" s="3">
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="14">
@@ -3164,16 +3257,19 @@
         <v>203.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3">
         <v>3.0</v>
       </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E14" s="3">
-        <v>160.0</v>
+        <v>9.0</v>
       </c>
       <c r="F14" s="3">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="15">
@@ -3181,16 +3277,19 @@
         <v>204.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3">
         <v>4.0</v>
       </c>
+      <c r="D15" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="E15" s="3">
-        <v>200.0</v>
+        <v>11.0</v>
       </c>
       <c r="F15" s="3">
-        <v>1.85</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="16">
@@ -3198,16 +3297,19 @@
         <v>205.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3">
         <v>5.0</v>
       </c>
+      <c r="D16" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="E16" s="3">
-        <v>240.0</v>
+        <v>13.0</v>
       </c>
       <c r="F16" s="3">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="17">
@@ -3215,16 +3317,19 @@
         <v>206.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3">
         <v>6.0</v>
       </c>
+      <c r="D17" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="E17" s="3">
-        <v>280.0</v>
+        <v>15.0</v>
       </c>
       <c r="F17" s="3">
-        <v>2.35</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="18">
@@ -3232,16 +3337,19 @@
         <v>207.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3">
         <v>7.0</v>
       </c>
+      <c r="D18" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="E18" s="3">
-        <v>320.0</v>
+        <v>17.0</v>
       </c>
       <c r="F18" s="3">
-        <v>2.6</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
@@ -3249,16 +3357,19 @@
         <v>208.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C19" s="3">
         <v>8.0</v>
       </c>
+      <c r="D19" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="E19" s="3">
-        <v>360.0</v>
+        <v>19.0</v>
       </c>
       <c r="F19" s="3">
-        <v>2.85</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="20">
@@ -3266,16 +3377,19 @@
         <v>209.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C20" s="3">
         <v>9.0</v>
       </c>
+      <c r="D20" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="E20" s="3">
-        <v>400.0</v>
+        <v>21.0</v>
       </c>
       <c r="F20" s="3">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="21">
@@ -3283,17 +3397,19 @@
         <v>210.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3">
         <v>10.0</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E21" s="3">
-        <v>440.0</v>
+        <v>23.0</v>
       </c>
       <c r="F21" s="3">
-        <v>3.35</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="22">
@@ -3301,19 +3417,19 @@
         <v>301.0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C22" s="3">
         <v>1.0</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>44</v>
+      <c r="D22" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="E22" s="3">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="F22" s="3">
-        <v>1.08</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="23">
@@ -3321,19 +3437,19 @@
         <v>302.0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C23" s="3">
         <v>2.0</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>45</v>
+      <c r="D23" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="E23" s="3">
-        <v>90.0</v>
+        <v>7.0</v>
       </c>
       <c r="F23" s="3">
-        <v>1.19</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="24">
@@ -3341,16 +3457,19 @@
         <v>303.0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C24" s="3">
         <v>3.0</v>
       </c>
+      <c r="D24" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="E24" s="3">
-        <v>130.0</v>
+        <v>9.0</v>
       </c>
       <c r="F24" s="3">
-        <v>1.3</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="25">
@@ -3358,16 +3477,19 @@
         <v>304.0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C25" s="3">
         <v>4.0</v>
       </c>
+      <c r="D25" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="E25" s="3">
-        <v>170.0</v>
+        <v>11.0</v>
       </c>
       <c r="F25" s="3">
-        <v>1.41</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="26">
@@ -3375,16 +3497,19 @@
         <v>305.0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C26" s="3">
         <v>5.0</v>
       </c>
+      <c r="D26" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="E26" s="3">
-        <v>210.0</v>
+        <v>13.0</v>
       </c>
       <c r="F26" s="3">
-        <v>1.52</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="27">
@@ -3392,16 +3517,19 @@
         <v>306.0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C27" s="3">
         <v>6.0</v>
       </c>
+      <c r="D27" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="E27" s="3">
-        <v>250.0</v>
+        <v>15.0</v>
       </c>
       <c r="F27" s="3">
-        <v>1.63</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="28">
@@ -3409,16 +3537,19 @@
         <v>307.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C28" s="3">
         <v>7.0</v>
       </c>
+      <c r="D28" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="E28" s="3">
-        <v>290.0</v>
+        <v>17.0</v>
       </c>
       <c r="F28" s="3">
-        <v>1.74</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="29">
@@ -3426,16 +3557,19 @@
         <v>308.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C29" s="3">
         <v>8.0</v>
       </c>
+      <c r="D29" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="E29" s="3">
-        <v>330.0</v>
+        <v>19.0</v>
       </c>
       <c r="F29" s="3">
-        <v>1.85</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="30">
@@ -3443,16 +3577,19 @@
         <v>309.0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C30" s="3">
         <v>9.0</v>
       </c>
+      <c r="D30" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="E30" s="3">
-        <v>370.0</v>
+        <v>21.0</v>
       </c>
       <c r="F30" s="3">
-        <v>1.96</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="31">
@@ -3460,16 +3597,19 @@
         <v>310.0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C31" s="3">
         <v>10.0</v>
       </c>
+      <c r="D31" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="E31" s="3">
-        <v>410.0</v>
+        <v>23.0</v>
       </c>
       <c r="F31" s="3">
-        <v>2.07</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="32">
@@ -3477,19 +3617,19 @@
         <v>401.0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C32" s="3">
         <v>1.0</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>47</v>
+      <c r="D32" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E32" s="3">
-        <v>150.0</v>
+        <v>5.0</v>
       </c>
       <c r="F32" s="3">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="33">
@@ -3497,19 +3637,19 @@
         <v>402.0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C33" s="3">
         <v>2.0</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>48</v>
+      <c r="D33" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="E33" s="3">
-        <v>200.0</v>
+        <v>7.0</v>
       </c>
       <c r="F33" s="3">
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="34">
@@ -3517,16 +3657,19 @@
         <v>403.0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C34" s="3">
         <v>3.0</v>
       </c>
+      <c r="D34" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="E34" s="3">
-        <v>250.0</v>
+        <v>9.0</v>
       </c>
       <c r="F34" s="3">
-        <v>2.2</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="35">
@@ -3534,16 +3677,19 @@
         <v>404.0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C35" s="3">
         <v>4.0</v>
       </c>
+      <c r="D35" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="E35" s="3">
-        <v>300.0</v>
+        <v>11.0</v>
       </c>
       <c r="F35" s="3">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="36">
@@ -3551,16 +3697,19 @@
         <v>405.0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3">
         <v>5.0</v>
       </c>
+      <c r="D36" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="E36" s="3">
-        <v>350.0</v>
+        <v>13.0</v>
       </c>
       <c r="F36" s="3">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="37">
@@ -3568,16 +3717,19 @@
         <v>406.0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C37" s="3">
         <v>6.0</v>
       </c>
+      <c r="D37" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="E37" s="3">
-        <v>400.0</v>
+        <v>15.0</v>
       </c>
       <c r="F37" s="3">
-        <v>3.1</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="38">
@@ -3585,16 +3737,19 @@
         <v>407.0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C38" s="3">
         <v>7.0</v>
       </c>
+      <c r="D38" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="E38" s="3">
-        <v>450.0</v>
+        <v>17.0</v>
       </c>
       <c r="F38" s="3">
-        <v>3.4</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="39">
@@ -3602,16 +3757,19 @@
         <v>408.0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C39" s="3">
         <v>8.0</v>
       </c>
+      <c r="D39" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="E39" s="3">
-        <v>500.0</v>
+        <v>19.0</v>
       </c>
       <c r="F39" s="3">
-        <v>3.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="40">
@@ -3619,16 +3777,19 @@
         <v>409.0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C40" s="3">
         <v>9.0</v>
       </c>
+      <c r="D40" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="E40" s="3">
-        <v>550.0</v>
+        <v>21.0</v>
       </c>
       <c r="F40" s="3">
-        <v>4.0</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="41">
@@ -3636,17 +3797,2918 @@
         <v>410.0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C41" s="3">
         <v>10.0</v>
       </c>
+      <c r="D41" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="E41" s="3">
-        <v>600.0</v>
+        <v>23.0</v>
       </c>
       <c r="F41" s="3">
-        <v>4.3</v>
-      </c>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43">
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44">
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45">
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46">
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47">
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48">
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49">
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50">
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51">
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52">
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53">
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54">
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55">
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56">
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57">
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58">
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59">
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60">
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61">
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62">
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63">
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64">
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65">
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66">
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67">
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68">
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69">
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70">
+      <c r="D70" s="7"/>
+    </row>
+    <row r="71">
+      <c r="D71" s="7"/>
+    </row>
+    <row r="72">
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73">
+      <c r="D73" s="7"/>
+    </row>
+    <row r="74">
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75">
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76">
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77">
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78">
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79">
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80">
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81">
+      <c r="D81" s="7"/>
+    </row>
+    <row r="82">
+      <c r="D82" s="7"/>
+    </row>
+    <row r="83">
+      <c r="D83" s="7"/>
+    </row>
+    <row r="84">
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85">
+      <c r="D85" s="7"/>
+    </row>
+    <row r="86">
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87">
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88">
+      <c r="D88" s="7"/>
+    </row>
+    <row r="89">
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90">
+      <c r="D90" s="7"/>
+    </row>
+    <row r="91">
+      <c r="D91" s="7"/>
+    </row>
+    <row r="92">
+      <c r="D92" s="7"/>
+    </row>
+    <row r="93">
+      <c r="D93" s="7"/>
+    </row>
+    <row r="94">
+      <c r="D94" s="7"/>
+    </row>
+    <row r="95">
+      <c r="D95" s="7"/>
+    </row>
+    <row r="96">
+      <c r="D96" s="7"/>
+    </row>
+    <row r="97">
+      <c r="D97" s="7"/>
+    </row>
+    <row r="98">
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99">
+      <c r="D99" s="7"/>
+    </row>
+    <row r="100">
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101">
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102">
+      <c r="D102" s="7"/>
+    </row>
+    <row r="103">
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104">
+      <c r="D104" s="7"/>
+    </row>
+    <row r="105">
+      <c r="D105" s="7"/>
+    </row>
+    <row r="106">
+      <c r="D106" s="7"/>
+    </row>
+    <row r="107">
+      <c r="D107" s="7"/>
+    </row>
+    <row r="108">
+      <c r="D108" s="7"/>
+    </row>
+    <row r="109">
+      <c r="D109" s="7"/>
+    </row>
+    <row r="110">
+      <c r="D110" s="7"/>
+    </row>
+    <row r="111">
+      <c r="D111" s="7"/>
+    </row>
+    <row r="112">
+      <c r="D112" s="7"/>
+    </row>
+    <row r="113">
+      <c r="D113" s="7"/>
+    </row>
+    <row r="114">
+      <c r="D114" s="7"/>
+    </row>
+    <row r="115">
+      <c r="D115" s="7"/>
+    </row>
+    <row r="116">
+      <c r="D116" s="7"/>
+    </row>
+    <row r="117">
+      <c r="D117" s="7"/>
+    </row>
+    <row r="118">
+      <c r="D118" s="7"/>
+    </row>
+    <row r="119">
+      <c r="D119" s="7"/>
+    </row>
+    <row r="120">
+      <c r="D120" s="7"/>
+    </row>
+    <row r="121">
+      <c r="D121" s="7"/>
+    </row>
+    <row r="122">
+      <c r="D122" s="7"/>
+    </row>
+    <row r="123">
+      <c r="D123" s="7"/>
+    </row>
+    <row r="124">
+      <c r="D124" s="7"/>
+    </row>
+    <row r="125">
+      <c r="D125" s="7"/>
+    </row>
+    <row r="126">
+      <c r="D126" s="7"/>
+    </row>
+    <row r="127">
+      <c r="D127" s="7"/>
+    </row>
+    <row r="128">
+      <c r="D128" s="7"/>
+    </row>
+    <row r="129">
+      <c r="D129" s="7"/>
+    </row>
+    <row r="130">
+      <c r="D130" s="7"/>
+    </row>
+    <row r="131">
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132">
+      <c r="D132" s="7"/>
+    </row>
+    <row r="133">
+      <c r="D133" s="7"/>
+    </row>
+    <row r="134">
+      <c r="D134" s="7"/>
+    </row>
+    <row r="135">
+      <c r="D135" s="7"/>
+    </row>
+    <row r="136">
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137">
+      <c r="D137" s="7"/>
+    </row>
+    <row r="138">
+      <c r="D138" s="7"/>
+    </row>
+    <row r="139">
+      <c r="D139" s="7"/>
+    </row>
+    <row r="140">
+      <c r="D140" s="7"/>
+    </row>
+    <row r="141">
+      <c r="D141" s="7"/>
+    </row>
+    <row r="142">
+      <c r="D142" s="7"/>
+    </row>
+    <row r="143">
+      <c r="D143" s="7"/>
+    </row>
+    <row r="144">
+      <c r="D144" s="7"/>
+    </row>
+    <row r="145">
+      <c r="D145" s="7"/>
+    </row>
+    <row r="146">
+      <c r="D146" s="7"/>
+    </row>
+    <row r="147">
+      <c r="D147" s="7"/>
+    </row>
+    <row r="148">
+      <c r="D148" s="7"/>
+    </row>
+    <row r="149">
+      <c r="D149" s="7"/>
+    </row>
+    <row r="150">
+      <c r="D150" s="7"/>
+    </row>
+    <row r="151">
+      <c r="D151" s="7"/>
+    </row>
+    <row r="152">
+      <c r="D152" s="7"/>
+    </row>
+    <row r="153">
+      <c r="D153" s="7"/>
+    </row>
+    <row r="154">
+      <c r="D154" s="7"/>
+    </row>
+    <row r="155">
+      <c r="D155" s="7"/>
+    </row>
+    <row r="156">
+      <c r="D156" s="7"/>
+    </row>
+    <row r="157">
+      <c r="D157" s="7"/>
+    </row>
+    <row r="158">
+      <c r="D158" s="7"/>
+    </row>
+    <row r="159">
+      <c r="D159" s="7"/>
+    </row>
+    <row r="160">
+      <c r="D160" s="7"/>
+    </row>
+    <row r="161">
+      <c r="D161" s="7"/>
+    </row>
+    <row r="162">
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163">
+      <c r="D163" s="7"/>
+    </row>
+    <row r="164">
+      <c r="D164" s="7"/>
+    </row>
+    <row r="165">
+      <c r="D165" s="7"/>
+    </row>
+    <row r="166">
+      <c r="D166" s="7"/>
+    </row>
+    <row r="167">
+      <c r="D167" s="7"/>
+    </row>
+    <row r="168">
+      <c r="D168" s="7"/>
+    </row>
+    <row r="169">
+      <c r="D169" s="7"/>
+    </row>
+    <row r="170">
+      <c r="D170" s="7"/>
+    </row>
+    <row r="171">
+      <c r="D171" s="7"/>
+    </row>
+    <row r="172">
+      <c r="D172" s="7"/>
+    </row>
+    <row r="173">
+      <c r="D173" s="7"/>
+    </row>
+    <row r="174">
+      <c r="D174" s="7"/>
+    </row>
+    <row r="175">
+      <c r="D175" s="7"/>
+    </row>
+    <row r="176">
+      <c r="D176" s="7"/>
+    </row>
+    <row r="177">
+      <c r="D177" s="7"/>
+    </row>
+    <row r="178">
+      <c r="D178" s="7"/>
+    </row>
+    <row r="179">
+      <c r="D179" s="7"/>
+    </row>
+    <row r="180">
+      <c r="D180" s="7"/>
+    </row>
+    <row r="181">
+      <c r="D181" s="7"/>
+    </row>
+    <row r="182">
+      <c r="D182" s="7"/>
+    </row>
+    <row r="183">
+      <c r="D183" s="7"/>
+    </row>
+    <row r="184">
+      <c r="D184" s="7"/>
+    </row>
+    <row r="185">
+      <c r="D185" s="7"/>
+    </row>
+    <row r="186">
+      <c r="D186" s="7"/>
+    </row>
+    <row r="187">
+      <c r="D187" s="7"/>
+    </row>
+    <row r="188">
+      <c r="D188" s="7"/>
+    </row>
+    <row r="189">
+      <c r="D189" s="7"/>
+    </row>
+    <row r="190">
+      <c r="D190" s="7"/>
+    </row>
+    <row r="191">
+      <c r="D191" s="7"/>
+    </row>
+    <row r="192">
+      <c r="D192" s="7"/>
+    </row>
+    <row r="193">
+      <c r="D193" s="7"/>
+    </row>
+    <row r="194">
+      <c r="D194" s="7"/>
+    </row>
+    <row r="195">
+      <c r="D195" s="7"/>
+    </row>
+    <row r="196">
+      <c r="D196" s="7"/>
+    </row>
+    <row r="197">
+      <c r="D197" s="7"/>
+    </row>
+    <row r="198">
+      <c r="D198" s="7"/>
+    </row>
+    <row r="199">
+      <c r="D199" s="7"/>
+    </row>
+    <row r="200">
+      <c r="D200" s="7"/>
+    </row>
+    <row r="201">
+      <c r="D201" s="7"/>
+    </row>
+    <row r="202">
+      <c r="D202" s="7"/>
+    </row>
+    <row r="203">
+      <c r="D203" s="7"/>
+    </row>
+    <row r="204">
+      <c r="D204" s="7"/>
+    </row>
+    <row r="205">
+      <c r="D205" s="7"/>
+    </row>
+    <row r="206">
+      <c r="D206" s="7"/>
+    </row>
+    <row r="207">
+      <c r="D207" s="7"/>
+    </row>
+    <row r="208">
+      <c r="D208" s="7"/>
+    </row>
+    <row r="209">
+      <c r="D209" s="7"/>
+    </row>
+    <row r="210">
+      <c r="D210" s="7"/>
+    </row>
+    <row r="211">
+      <c r="D211" s="7"/>
+    </row>
+    <row r="212">
+      <c r="D212" s="7"/>
+    </row>
+    <row r="213">
+      <c r="D213" s="7"/>
+    </row>
+    <row r="214">
+      <c r="D214" s="7"/>
+    </row>
+    <row r="215">
+      <c r="D215" s="7"/>
+    </row>
+    <row r="216">
+      <c r="D216" s="7"/>
+    </row>
+    <row r="217">
+      <c r="D217" s="7"/>
+    </row>
+    <row r="218">
+      <c r="D218" s="7"/>
+    </row>
+    <row r="219">
+      <c r="D219" s="7"/>
+    </row>
+    <row r="220">
+      <c r="D220" s="7"/>
+    </row>
+    <row r="221">
+      <c r="D221" s="7"/>
+    </row>
+    <row r="222">
+      <c r="D222" s="7"/>
+    </row>
+    <row r="223">
+      <c r="D223" s="7"/>
+    </row>
+    <row r="224">
+      <c r="D224" s="7"/>
+    </row>
+    <row r="225">
+      <c r="D225" s="7"/>
+    </row>
+    <row r="226">
+      <c r="D226" s="7"/>
+    </row>
+    <row r="227">
+      <c r="D227" s="7"/>
+    </row>
+    <row r="228">
+      <c r="D228" s="7"/>
+    </row>
+    <row r="229">
+      <c r="D229" s="7"/>
+    </row>
+    <row r="230">
+      <c r="D230" s="7"/>
+    </row>
+    <row r="231">
+      <c r="D231" s="7"/>
+    </row>
+    <row r="232">
+      <c r="D232" s="7"/>
+    </row>
+    <row r="233">
+      <c r="D233" s="7"/>
+    </row>
+    <row r="234">
+      <c r="D234" s="7"/>
+    </row>
+    <row r="235">
+      <c r="D235" s="7"/>
+    </row>
+    <row r="236">
+      <c r="D236" s="7"/>
+    </row>
+    <row r="237">
+      <c r="D237" s="7"/>
+    </row>
+    <row r="238">
+      <c r="D238" s="7"/>
+    </row>
+    <row r="239">
+      <c r="D239" s="7"/>
+    </row>
+    <row r="240">
+      <c r="D240" s="7"/>
+    </row>
+    <row r="241">
+      <c r="D241" s="7"/>
+    </row>
+    <row r="242">
+      <c r="D242" s="7"/>
+    </row>
+    <row r="243">
+      <c r="D243" s="7"/>
+    </row>
+    <row r="244">
+      <c r="D244" s="7"/>
+    </row>
+    <row r="245">
+      <c r="D245" s="7"/>
+    </row>
+    <row r="246">
+      <c r="D246" s="7"/>
+    </row>
+    <row r="247">
+      <c r="D247" s="7"/>
+    </row>
+    <row r="248">
+      <c r="D248" s="7"/>
+    </row>
+    <row r="249">
+      <c r="D249" s="7"/>
+    </row>
+    <row r="250">
+      <c r="D250" s="7"/>
+    </row>
+    <row r="251">
+      <c r="D251" s="7"/>
+    </row>
+    <row r="252">
+      <c r="D252" s="7"/>
+    </row>
+    <row r="253">
+      <c r="D253" s="7"/>
+    </row>
+    <row r="254">
+      <c r="D254" s="7"/>
+    </row>
+    <row r="255">
+      <c r="D255" s="7"/>
+    </row>
+    <row r="256">
+      <c r="D256" s="7"/>
+    </row>
+    <row r="257">
+      <c r="D257" s="7"/>
+    </row>
+    <row r="258">
+      <c r="D258" s="7"/>
+    </row>
+    <row r="259">
+      <c r="D259" s="7"/>
+    </row>
+    <row r="260">
+      <c r="D260" s="7"/>
+    </row>
+    <row r="261">
+      <c r="D261" s="7"/>
+    </row>
+    <row r="262">
+      <c r="D262" s="7"/>
+    </row>
+    <row r="263">
+      <c r="D263" s="7"/>
+    </row>
+    <row r="264">
+      <c r="D264" s="7"/>
+    </row>
+    <row r="265">
+      <c r="D265" s="7"/>
+    </row>
+    <row r="266">
+      <c r="D266" s="7"/>
+    </row>
+    <row r="267">
+      <c r="D267" s="7"/>
+    </row>
+    <row r="268">
+      <c r="D268" s="7"/>
+    </row>
+    <row r="269">
+      <c r="D269" s="7"/>
+    </row>
+    <row r="270">
+      <c r="D270" s="7"/>
+    </row>
+    <row r="271">
+      <c r="D271" s="7"/>
+    </row>
+    <row r="272">
+      <c r="D272" s="7"/>
+    </row>
+    <row r="273">
+      <c r="D273" s="7"/>
+    </row>
+    <row r="274">
+      <c r="D274" s="7"/>
+    </row>
+    <row r="275">
+      <c r="D275" s="7"/>
+    </row>
+    <row r="276">
+      <c r="D276" s="7"/>
+    </row>
+    <row r="277">
+      <c r="D277" s="7"/>
+    </row>
+    <row r="278">
+      <c r="D278" s="7"/>
+    </row>
+    <row r="279">
+      <c r="D279" s="7"/>
+    </row>
+    <row r="280">
+      <c r="D280" s="7"/>
+    </row>
+    <row r="281">
+      <c r="D281" s="7"/>
+    </row>
+    <row r="282">
+      <c r="D282" s="7"/>
+    </row>
+    <row r="283">
+      <c r="D283" s="7"/>
+    </row>
+    <row r="284">
+      <c r="D284" s="7"/>
+    </row>
+    <row r="285">
+      <c r="D285" s="7"/>
+    </row>
+    <row r="286">
+      <c r="D286" s="7"/>
+    </row>
+    <row r="287">
+      <c r="D287" s="7"/>
+    </row>
+    <row r="288">
+      <c r="D288" s="7"/>
+    </row>
+    <row r="289">
+      <c r="D289" s="7"/>
+    </row>
+    <row r="290">
+      <c r="D290" s="7"/>
+    </row>
+    <row r="291">
+      <c r="D291" s="7"/>
+    </row>
+    <row r="292">
+      <c r="D292" s="7"/>
+    </row>
+    <row r="293">
+      <c r="D293" s="7"/>
+    </row>
+    <row r="294">
+      <c r="D294" s="7"/>
+    </row>
+    <row r="295">
+      <c r="D295" s="7"/>
+    </row>
+    <row r="296">
+      <c r="D296" s="7"/>
+    </row>
+    <row r="297">
+      <c r="D297" s="7"/>
+    </row>
+    <row r="298">
+      <c r="D298" s="7"/>
+    </row>
+    <row r="299">
+      <c r="D299" s="7"/>
+    </row>
+    <row r="300">
+      <c r="D300" s="7"/>
+    </row>
+    <row r="301">
+      <c r="D301" s="7"/>
+    </row>
+    <row r="302">
+      <c r="D302" s="7"/>
+    </row>
+    <row r="303">
+      <c r="D303" s="7"/>
+    </row>
+    <row r="304">
+      <c r="D304" s="7"/>
+    </row>
+    <row r="305">
+      <c r="D305" s="7"/>
+    </row>
+    <row r="306">
+      <c r="D306" s="7"/>
+    </row>
+    <row r="307">
+      <c r="D307" s="7"/>
+    </row>
+    <row r="308">
+      <c r="D308" s="7"/>
+    </row>
+    <row r="309">
+      <c r="D309" s="7"/>
+    </row>
+    <row r="310">
+      <c r="D310" s="7"/>
+    </row>
+    <row r="311">
+      <c r="D311" s="7"/>
+    </row>
+    <row r="312">
+      <c r="D312" s="7"/>
+    </row>
+    <row r="313">
+      <c r="D313" s="7"/>
+    </row>
+    <row r="314">
+      <c r="D314" s="7"/>
+    </row>
+    <row r="315">
+      <c r="D315" s="7"/>
+    </row>
+    <row r="316">
+      <c r="D316" s="7"/>
+    </row>
+    <row r="317">
+      <c r="D317" s="7"/>
+    </row>
+    <row r="318">
+      <c r="D318" s="7"/>
+    </row>
+    <row r="319">
+      <c r="D319" s="7"/>
+    </row>
+    <row r="320">
+      <c r="D320" s="7"/>
+    </row>
+    <row r="321">
+      <c r="D321" s="7"/>
+    </row>
+    <row r="322">
+      <c r="D322" s="7"/>
+    </row>
+    <row r="323">
+      <c r="D323" s="7"/>
+    </row>
+    <row r="324">
+      <c r="D324" s="7"/>
+    </row>
+    <row r="325">
+      <c r="D325" s="7"/>
+    </row>
+    <row r="326">
+      <c r="D326" s="7"/>
+    </row>
+    <row r="327">
+      <c r="D327" s="7"/>
+    </row>
+    <row r="328">
+      <c r="D328" s="7"/>
+    </row>
+    <row r="329">
+      <c r="D329" s="7"/>
+    </row>
+    <row r="330">
+      <c r="D330" s="7"/>
+    </row>
+    <row r="331">
+      <c r="D331" s="7"/>
+    </row>
+    <row r="332">
+      <c r="D332" s="7"/>
+    </row>
+    <row r="333">
+      <c r="D333" s="7"/>
+    </row>
+    <row r="334">
+      <c r="D334" s="7"/>
+    </row>
+    <row r="335">
+      <c r="D335" s="7"/>
+    </row>
+    <row r="336">
+      <c r="D336" s="7"/>
+    </row>
+    <row r="337">
+      <c r="D337" s="7"/>
+    </row>
+    <row r="338">
+      <c r="D338" s="7"/>
+    </row>
+    <row r="339">
+      <c r="D339" s="7"/>
+    </row>
+    <row r="340">
+      <c r="D340" s="7"/>
+    </row>
+    <row r="341">
+      <c r="D341" s="7"/>
+    </row>
+    <row r="342">
+      <c r="D342" s="7"/>
+    </row>
+    <row r="343">
+      <c r="D343" s="7"/>
+    </row>
+    <row r="344">
+      <c r="D344" s="7"/>
+    </row>
+    <row r="345">
+      <c r="D345" s="7"/>
+    </row>
+    <row r="346">
+      <c r="D346" s="7"/>
+    </row>
+    <row r="347">
+      <c r="D347" s="7"/>
+    </row>
+    <row r="348">
+      <c r="D348" s="7"/>
+    </row>
+    <row r="349">
+      <c r="D349" s="7"/>
+    </row>
+    <row r="350">
+      <c r="D350" s="7"/>
+    </row>
+    <row r="351">
+      <c r="D351" s="7"/>
+    </row>
+    <row r="352">
+      <c r="D352" s="7"/>
+    </row>
+    <row r="353">
+      <c r="D353" s="7"/>
+    </row>
+    <row r="354">
+      <c r="D354" s="7"/>
+    </row>
+    <row r="355">
+      <c r="D355" s="7"/>
+    </row>
+    <row r="356">
+      <c r="D356" s="7"/>
+    </row>
+    <row r="357">
+      <c r="D357" s="7"/>
+    </row>
+    <row r="358">
+      <c r="D358" s="7"/>
+    </row>
+    <row r="359">
+      <c r="D359" s="7"/>
+    </row>
+    <row r="360">
+      <c r="D360" s="7"/>
+    </row>
+    <row r="361">
+      <c r="D361" s="7"/>
+    </row>
+    <row r="362">
+      <c r="D362" s="7"/>
+    </row>
+    <row r="363">
+      <c r="D363" s="7"/>
+    </row>
+    <row r="364">
+      <c r="D364" s="7"/>
+    </row>
+    <row r="365">
+      <c r="D365" s="7"/>
+    </row>
+    <row r="366">
+      <c r="D366" s="7"/>
+    </row>
+    <row r="367">
+      <c r="D367" s="7"/>
+    </row>
+    <row r="368">
+      <c r="D368" s="7"/>
+    </row>
+    <row r="369">
+      <c r="D369" s="7"/>
+    </row>
+    <row r="370">
+      <c r="D370" s="7"/>
+    </row>
+    <row r="371">
+      <c r="D371" s="7"/>
+    </row>
+    <row r="372">
+      <c r="D372" s="7"/>
+    </row>
+    <row r="373">
+      <c r="D373" s="7"/>
+    </row>
+    <row r="374">
+      <c r="D374" s="7"/>
+    </row>
+    <row r="375">
+      <c r="D375" s="7"/>
+    </row>
+    <row r="376">
+      <c r="D376" s="7"/>
+    </row>
+    <row r="377">
+      <c r="D377" s="7"/>
+    </row>
+    <row r="378">
+      <c r="D378" s="7"/>
+    </row>
+    <row r="379">
+      <c r="D379" s="7"/>
+    </row>
+    <row r="380">
+      <c r="D380" s="7"/>
+    </row>
+    <row r="381">
+      <c r="D381" s="7"/>
+    </row>
+    <row r="382">
+      <c r="D382" s="7"/>
+    </row>
+    <row r="383">
+      <c r="D383" s="7"/>
+    </row>
+    <row r="384">
+      <c r="D384" s="7"/>
+    </row>
+    <row r="385">
+      <c r="D385" s="7"/>
+    </row>
+    <row r="386">
+      <c r="D386" s="7"/>
+    </row>
+    <row r="387">
+      <c r="D387" s="7"/>
+    </row>
+    <row r="388">
+      <c r="D388" s="7"/>
+    </row>
+    <row r="389">
+      <c r="D389" s="7"/>
+    </row>
+    <row r="390">
+      <c r="D390" s="7"/>
+    </row>
+    <row r="391">
+      <c r="D391" s="7"/>
+    </row>
+    <row r="392">
+      <c r="D392" s="7"/>
+    </row>
+    <row r="393">
+      <c r="D393" s="7"/>
+    </row>
+    <row r="394">
+      <c r="D394" s="7"/>
+    </row>
+    <row r="395">
+      <c r="D395" s="7"/>
+    </row>
+    <row r="396">
+      <c r="D396" s="7"/>
+    </row>
+    <row r="397">
+      <c r="D397" s="7"/>
+    </row>
+    <row r="398">
+      <c r="D398" s="7"/>
+    </row>
+    <row r="399">
+      <c r="D399" s="7"/>
+    </row>
+    <row r="400">
+      <c r="D400" s="7"/>
+    </row>
+    <row r="401">
+      <c r="D401" s="7"/>
+    </row>
+    <row r="402">
+      <c r="D402" s="7"/>
+    </row>
+    <row r="403">
+      <c r="D403" s="7"/>
+    </row>
+    <row r="404">
+      <c r="D404" s="7"/>
+    </row>
+    <row r="405">
+      <c r="D405" s="7"/>
+    </row>
+    <row r="406">
+      <c r="D406" s="7"/>
+    </row>
+    <row r="407">
+      <c r="D407" s="7"/>
+    </row>
+    <row r="408">
+      <c r="D408" s="7"/>
+    </row>
+    <row r="409">
+      <c r="D409" s="7"/>
+    </row>
+    <row r="410">
+      <c r="D410" s="7"/>
+    </row>
+    <row r="411">
+      <c r="D411" s="7"/>
+    </row>
+    <row r="412">
+      <c r="D412" s="7"/>
+    </row>
+    <row r="413">
+      <c r="D413" s="7"/>
+    </row>
+    <row r="414">
+      <c r="D414" s="7"/>
+    </row>
+    <row r="415">
+      <c r="D415" s="7"/>
+    </row>
+    <row r="416">
+      <c r="D416" s="7"/>
+    </row>
+    <row r="417">
+      <c r="D417" s="7"/>
+    </row>
+    <row r="418">
+      <c r="D418" s="7"/>
+    </row>
+    <row r="419">
+      <c r="D419" s="7"/>
+    </row>
+    <row r="420">
+      <c r="D420" s="7"/>
+    </row>
+    <row r="421">
+      <c r="D421" s="7"/>
+    </row>
+    <row r="422">
+      <c r="D422" s="7"/>
+    </row>
+    <row r="423">
+      <c r="D423" s="7"/>
+    </row>
+    <row r="424">
+      <c r="D424" s="7"/>
+    </row>
+    <row r="425">
+      <c r="D425" s="7"/>
+    </row>
+    <row r="426">
+      <c r="D426" s="7"/>
+    </row>
+    <row r="427">
+      <c r="D427" s="7"/>
+    </row>
+    <row r="428">
+      <c r="D428" s="7"/>
+    </row>
+    <row r="429">
+      <c r="D429" s="7"/>
+    </row>
+    <row r="430">
+      <c r="D430" s="7"/>
+    </row>
+    <row r="431">
+      <c r="D431" s="7"/>
+    </row>
+    <row r="432">
+      <c r="D432" s="7"/>
+    </row>
+    <row r="433">
+      <c r="D433" s="7"/>
+    </row>
+    <row r="434">
+      <c r="D434" s="7"/>
+    </row>
+    <row r="435">
+      <c r="D435" s="7"/>
+    </row>
+    <row r="436">
+      <c r="D436" s="7"/>
+    </row>
+    <row r="437">
+      <c r="D437" s="7"/>
+    </row>
+    <row r="438">
+      <c r="D438" s="7"/>
+    </row>
+    <row r="439">
+      <c r="D439" s="7"/>
+    </row>
+    <row r="440">
+      <c r="D440" s="7"/>
+    </row>
+    <row r="441">
+      <c r="D441" s="7"/>
+    </row>
+    <row r="442">
+      <c r="D442" s="7"/>
+    </row>
+    <row r="443">
+      <c r="D443" s="7"/>
+    </row>
+    <row r="444">
+      <c r="D444" s="7"/>
+    </row>
+    <row r="445">
+      <c r="D445" s="7"/>
+    </row>
+    <row r="446">
+      <c r="D446" s="7"/>
+    </row>
+    <row r="447">
+      <c r="D447" s="7"/>
+    </row>
+    <row r="448">
+      <c r="D448" s="7"/>
+    </row>
+    <row r="449">
+      <c r="D449" s="7"/>
+    </row>
+    <row r="450">
+      <c r="D450" s="7"/>
+    </row>
+    <row r="451">
+      <c r="D451" s="7"/>
+    </row>
+    <row r="452">
+      <c r="D452" s="7"/>
+    </row>
+    <row r="453">
+      <c r="D453" s="7"/>
+    </row>
+    <row r="454">
+      <c r="D454" s="7"/>
+    </row>
+    <row r="455">
+      <c r="D455" s="7"/>
+    </row>
+    <row r="456">
+      <c r="D456" s="7"/>
+    </row>
+    <row r="457">
+      <c r="D457" s="7"/>
+    </row>
+    <row r="458">
+      <c r="D458" s="7"/>
+    </row>
+    <row r="459">
+      <c r="D459" s="7"/>
+    </row>
+    <row r="460">
+      <c r="D460" s="7"/>
+    </row>
+    <row r="461">
+      <c r="D461" s="7"/>
+    </row>
+    <row r="462">
+      <c r="D462" s="7"/>
+    </row>
+    <row r="463">
+      <c r="D463" s="7"/>
+    </row>
+    <row r="464">
+      <c r="D464" s="7"/>
+    </row>
+    <row r="465">
+      <c r="D465" s="7"/>
+    </row>
+    <row r="466">
+      <c r="D466" s="7"/>
+    </row>
+    <row r="467">
+      <c r="D467" s="7"/>
+    </row>
+    <row r="468">
+      <c r="D468" s="7"/>
+    </row>
+    <row r="469">
+      <c r="D469" s="7"/>
+    </row>
+    <row r="470">
+      <c r="D470" s="7"/>
+    </row>
+    <row r="471">
+      <c r="D471" s="7"/>
+    </row>
+    <row r="472">
+      <c r="D472" s="7"/>
+    </row>
+    <row r="473">
+      <c r="D473" s="7"/>
+    </row>
+    <row r="474">
+      <c r="D474" s="7"/>
+    </row>
+    <row r="475">
+      <c r="D475" s="7"/>
+    </row>
+    <row r="476">
+      <c r="D476" s="7"/>
+    </row>
+    <row r="477">
+      <c r="D477" s="7"/>
+    </row>
+    <row r="478">
+      <c r="D478" s="7"/>
+    </row>
+    <row r="479">
+      <c r="D479" s="7"/>
+    </row>
+    <row r="480">
+      <c r="D480" s="7"/>
+    </row>
+    <row r="481">
+      <c r="D481" s="7"/>
+    </row>
+    <row r="482">
+      <c r="D482" s="7"/>
+    </row>
+    <row r="483">
+      <c r="D483" s="7"/>
+    </row>
+    <row r="484">
+      <c r="D484" s="7"/>
+    </row>
+    <row r="485">
+      <c r="D485" s="7"/>
+    </row>
+    <row r="486">
+      <c r="D486" s="7"/>
+    </row>
+    <row r="487">
+      <c r="D487" s="7"/>
+    </row>
+    <row r="488">
+      <c r="D488" s="7"/>
+    </row>
+    <row r="489">
+      <c r="D489" s="7"/>
+    </row>
+    <row r="490">
+      <c r="D490" s="7"/>
+    </row>
+    <row r="491">
+      <c r="D491" s="7"/>
+    </row>
+    <row r="492">
+      <c r="D492" s="7"/>
+    </row>
+    <row r="493">
+      <c r="D493" s="7"/>
+    </row>
+    <row r="494">
+      <c r="D494" s="7"/>
+    </row>
+    <row r="495">
+      <c r="D495" s="7"/>
+    </row>
+    <row r="496">
+      <c r="D496" s="7"/>
+    </row>
+    <row r="497">
+      <c r="D497" s="7"/>
+    </row>
+    <row r="498">
+      <c r="D498" s="7"/>
+    </row>
+    <row r="499">
+      <c r="D499" s="7"/>
+    </row>
+    <row r="500">
+      <c r="D500" s="7"/>
+    </row>
+    <row r="501">
+      <c r="D501" s="7"/>
+    </row>
+    <row r="502">
+      <c r="D502" s="7"/>
+    </row>
+    <row r="503">
+      <c r="D503" s="7"/>
+    </row>
+    <row r="504">
+      <c r="D504" s="7"/>
+    </row>
+    <row r="505">
+      <c r="D505" s="7"/>
+    </row>
+    <row r="506">
+      <c r="D506" s="7"/>
+    </row>
+    <row r="507">
+      <c r="D507" s="7"/>
+    </row>
+    <row r="508">
+      <c r="D508" s="7"/>
+    </row>
+    <row r="509">
+      <c r="D509" s="7"/>
+    </row>
+    <row r="510">
+      <c r="D510" s="7"/>
+    </row>
+    <row r="511">
+      <c r="D511" s="7"/>
+    </row>
+    <row r="512">
+      <c r="D512" s="7"/>
+    </row>
+    <row r="513">
+      <c r="D513" s="7"/>
+    </row>
+    <row r="514">
+      <c r="D514" s="7"/>
+    </row>
+    <row r="515">
+      <c r="D515" s="7"/>
+    </row>
+    <row r="516">
+      <c r="D516" s="7"/>
+    </row>
+    <row r="517">
+      <c r="D517" s="7"/>
+    </row>
+    <row r="518">
+      <c r="D518" s="7"/>
+    </row>
+    <row r="519">
+      <c r="D519" s="7"/>
+    </row>
+    <row r="520">
+      <c r="D520" s="7"/>
+    </row>
+    <row r="521">
+      <c r="D521" s="7"/>
+    </row>
+    <row r="522">
+      <c r="D522" s="7"/>
+    </row>
+    <row r="523">
+      <c r="D523" s="7"/>
+    </row>
+    <row r="524">
+      <c r="D524" s="7"/>
+    </row>
+    <row r="525">
+      <c r="D525" s="7"/>
+    </row>
+    <row r="526">
+      <c r="D526" s="7"/>
+    </row>
+    <row r="527">
+      <c r="D527" s="7"/>
+    </row>
+    <row r="528">
+      <c r="D528" s="7"/>
+    </row>
+    <row r="529">
+      <c r="D529" s="7"/>
+    </row>
+    <row r="530">
+      <c r="D530" s="7"/>
+    </row>
+    <row r="531">
+      <c r="D531" s="7"/>
+    </row>
+    <row r="532">
+      <c r="D532" s="7"/>
+    </row>
+    <row r="533">
+      <c r="D533" s="7"/>
+    </row>
+    <row r="534">
+      <c r="D534" s="7"/>
+    </row>
+    <row r="535">
+      <c r="D535" s="7"/>
+    </row>
+    <row r="536">
+      <c r="D536" s="7"/>
+    </row>
+    <row r="537">
+      <c r="D537" s="7"/>
+    </row>
+    <row r="538">
+      <c r="D538" s="7"/>
+    </row>
+    <row r="539">
+      <c r="D539" s="7"/>
+    </row>
+    <row r="540">
+      <c r="D540" s="7"/>
+    </row>
+    <row r="541">
+      <c r="D541" s="7"/>
+    </row>
+    <row r="542">
+      <c r="D542" s="7"/>
+    </row>
+    <row r="543">
+      <c r="D543" s="7"/>
+    </row>
+    <row r="544">
+      <c r="D544" s="7"/>
+    </row>
+    <row r="545">
+      <c r="D545" s="7"/>
+    </row>
+    <row r="546">
+      <c r="D546" s="7"/>
+    </row>
+    <row r="547">
+      <c r="D547" s="7"/>
+    </row>
+    <row r="548">
+      <c r="D548" s="7"/>
+    </row>
+    <row r="549">
+      <c r="D549" s="7"/>
+    </row>
+    <row r="550">
+      <c r="D550" s="7"/>
+    </row>
+    <row r="551">
+      <c r="D551" s="7"/>
+    </row>
+    <row r="552">
+      <c r="D552" s="7"/>
+    </row>
+    <row r="553">
+      <c r="D553" s="7"/>
+    </row>
+    <row r="554">
+      <c r="D554" s="7"/>
+    </row>
+    <row r="555">
+      <c r="D555" s="7"/>
+    </row>
+    <row r="556">
+      <c r="D556" s="7"/>
+    </row>
+    <row r="557">
+      <c r="D557" s="7"/>
+    </row>
+    <row r="558">
+      <c r="D558" s="7"/>
+    </row>
+    <row r="559">
+      <c r="D559" s="7"/>
+    </row>
+    <row r="560">
+      <c r="D560" s="7"/>
+    </row>
+    <row r="561">
+      <c r="D561" s="7"/>
+    </row>
+    <row r="562">
+      <c r="D562" s="7"/>
+    </row>
+    <row r="563">
+      <c r="D563" s="7"/>
+    </row>
+    <row r="564">
+      <c r="D564" s="7"/>
+    </row>
+    <row r="565">
+      <c r="D565" s="7"/>
+    </row>
+    <row r="566">
+      <c r="D566" s="7"/>
+    </row>
+    <row r="567">
+      <c r="D567" s="7"/>
+    </row>
+    <row r="568">
+      <c r="D568" s="7"/>
+    </row>
+    <row r="569">
+      <c r="D569" s="7"/>
+    </row>
+    <row r="570">
+      <c r="D570" s="7"/>
+    </row>
+    <row r="571">
+      <c r="D571" s="7"/>
+    </row>
+    <row r="572">
+      <c r="D572" s="7"/>
+    </row>
+    <row r="573">
+      <c r="D573" s="7"/>
+    </row>
+    <row r="574">
+      <c r="D574" s="7"/>
+    </row>
+    <row r="575">
+      <c r="D575" s="7"/>
+    </row>
+    <row r="576">
+      <c r="D576" s="7"/>
+    </row>
+    <row r="577">
+      <c r="D577" s="7"/>
+    </row>
+    <row r="578">
+      <c r="D578" s="7"/>
+    </row>
+    <row r="579">
+      <c r="D579" s="7"/>
+    </row>
+    <row r="580">
+      <c r="D580" s="7"/>
+    </row>
+    <row r="581">
+      <c r="D581" s="7"/>
+    </row>
+    <row r="582">
+      <c r="D582" s="7"/>
+    </row>
+    <row r="583">
+      <c r="D583" s="7"/>
+    </row>
+    <row r="584">
+      <c r="D584" s="7"/>
+    </row>
+    <row r="585">
+      <c r="D585" s="7"/>
+    </row>
+    <row r="586">
+      <c r="D586" s="7"/>
+    </row>
+    <row r="587">
+      <c r="D587" s="7"/>
+    </row>
+    <row r="588">
+      <c r="D588" s="7"/>
+    </row>
+    <row r="589">
+      <c r="D589" s="7"/>
+    </row>
+    <row r="590">
+      <c r="D590" s="7"/>
+    </row>
+    <row r="591">
+      <c r="D591" s="7"/>
+    </row>
+    <row r="592">
+      <c r="D592" s="7"/>
+    </row>
+    <row r="593">
+      <c r="D593" s="7"/>
+    </row>
+    <row r="594">
+      <c r="D594" s="7"/>
+    </row>
+    <row r="595">
+      <c r="D595" s="7"/>
+    </row>
+    <row r="596">
+      <c r="D596" s="7"/>
+    </row>
+    <row r="597">
+      <c r="D597" s="7"/>
+    </row>
+    <row r="598">
+      <c r="D598" s="7"/>
+    </row>
+    <row r="599">
+      <c r="D599" s="7"/>
+    </row>
+    <row r="600">
+      <c r="D600" s="7"/>
+    </row>
+    <row r="601">
+      <c r="D601" s="7"/>
+    </row>
+    <row r="602">
+      <c r="D602" s="7"/>
+    </row>
+    <row r="603">
+      <c r="D603" s="7"/>
+    </row>
+    <row r="604">
+      <c r="D604" s="7"/>
+    </row>
+    <row r="605">
+      <c r="D605" s="7"/>
+    </row>
+    <row r="606">
+      <c r="D606" s="7"/>
+    </row>
+    <row r="607">
+      <c r="D607" s="7"/>
+    </row>
+    <row r="608">
+      <c r="D608" s="7"/>
+    </row>
+    <row r="609">
+      <c r="D609" s="7"/>
+    </row>
+    <row r="610">
+      <c r="D610" s="7"/>
+    </row>
+    <row r="611">
+      <c r="D611" s="7"/>
+    </row>
+    <row r="612">
+      <c r="D612" s="7"/>
+    </row>
+    <row r="613">
+      <c r="D613" s="7"/>
+    </row>
+    <row r="614">
+      <c r="D614" s="7"/>
+    </row>
+    <row r="615">
+      <c r="D615" s="7"/>
+    </row>
+    <row r="616">
+      <c r="D616" s="7"/>
+    </row>
+    <row r="617">
+      <c r="D617" s="7"/>
+    </row>
+    <row r="618">
+      <c r="D618" s="7"/>
+    </row>
+    <row r="619">
+      <c r="D619" s="7"/>
+    </row>
+    <row r="620">
+      <c r="D620" s="7"/>
+    </row>
+    <row r="621">
+      <c r="D621" s="7"/>
+    </row>
+    <row r="622">
+      <c r="D622" s="7"/>
+    </row>
+    <row r="623">
+      <c r="D623" s="7"/>
+    </row>
+    <row r="624">
+      <c r="D624" s="7"/>
+    </row>
+    <row r="625">
+      <c r="D625" s="7"/>
+    </row>
+    <row r="626">
+      <c r="D626" s="7"/>
+    </row>
+    <row r="627">
+      <c r="D627" s="7"/>
+    </row>
+    <row r="628">
+      <c r="D628" s="7"/>
+    </row>
+    <row r="629">
+      <c r="D629" s="7"/>
+    </row>
+    <row r="630">
+      <c r="D630" s="7"/>
+    </row>
+    <row r="631">
+      <c r="D631" s="7"/>
+    </row>
+    <row r="632">
+      <c r="D632" s="7"/>
+    </row>
+    <row r="633">
+      <c r="D633" s="7"/>
+    </row>
+    <row r="634">
+      <c r="D634" s="7"/>
+    </row>
+    <row r="635">
+      <c r="D635" s="7"/>
+    </row>
+    <row r="636">
+      <c r="D636" s="7"/>
+    </row>
+    <row r="637">
+      <c r="D637" s="7"/>
+    </row>
+    <row r="638">
+      <c r="D638" s="7"/>
+    </row>
+    <row r="639">
+      <c r="D639" s="7"/>
+    </row>
+    <row r="640">
+      <c r="D640" s="7"/>
+    </row>
+    <row r="641">
+      <c r="D641" s="7"/>
+    </row>
+    <row r="642">
+      <c r="D642" s="7"/>
+    </row>
+    <row r="643">
+      <c r="D643" s="7"/>
+    </row>
+    <row r="644">
+      <c r="D644" s="7"/>
+    </row>
+    <row r="645">
+      <c r="D645" s="7"/>
+    </row>
+    <row r="646">
+      <c r="D646" s="7"/>
+    </row>
+    <row r="647">
+      <c r="D647" s="7"/>
+    </row>
+    <row r="648">
+      <c r="D648" s="7"/>
+    </row>
+    <row r="649">
+      <c r="D649" s="7"/>
+    </row>
+    <row r="650">
+      <c r="D650" s="7"/>
+    </row>
+    <row r="651">
+      <c r="D651" s="7"/>
+    </row>
+    <row r="652">
+      <c r="D652" s="7"/>
+    </row>
+    <row r="653">
+      <c r="D653" s="7"/>
+    </row>
+    <row r="654">
+      <c r="D654" s="7"/>
+    </row>
+    <row r="655">
+      <c r="D655" s="7"/>
+    </row>
+    <row r="656">
+      <c r="D656" s="7"/>
+    </row>
+    <row r="657">
+      <c r="D657" s="7"/>
+    </row>
+    <row r="658">
+      <c r="D658" s="7"/>
+    </row>
+    <row r="659">
+      <c r="D659" s="7"/>
+    </row>
+    <row r="660">
+      <c r="D660" s="7"/>
+    </row>
+    <row r="661">
+      <c r="D661" s="7"/>
+    </row>
+    <row r="662">
+      <c r="D662" s="7"/>
+    </row>
+    <row r="663">
+      <c r="D663" s="7"/>
+    </row>
+    <row r="664">
+      <c r="D664" s="7"/>
+    </row>
+    <row r="665">
+      <c r="D665" s="7"/>
+    </row>
+    <row r="666">
+      <c r="D666" s="7"/>
+    </row>
+    <row r="667">
+      <c r="D667" s="7"/>
+    </row>
+    <row r="668">
+      <c r="D668" s="7"/>
+    </row>
+    <row r="669">
+      <c r="D669" s="7"/>
+    </row>
+    <row r="670">
+      <c r="D670" s="7"/>
+    </row>
+    <row r="671">
+      <c r="D671" s="7"/>
+    </row>
+    <row r="672">
+      <c r="D672" s="7"/>
+    </row>
+    <row r="673">
+      <c r="D673" s="7"/>
+    </row>
+    <row r="674">
+      <c r="D674" s="7"/>
+    </row>
+    <row r="675">
+      <c r="D675" s="7"/>
+    </row>
+    <row r="676">
+      <c r="D676" s="7"/>
+    </row>
+    <row r="677">
+      <c r="D677" s="7"/>
+    </row>
+    <row r="678">
+      <c r="D678" s="7"/>
+    </row>
+    <row r="679">
+      <c r="D679" s="7"/>
+    </row>
+    <row r="680">
+      <c r="D680" s="7"/>
+    </row>
+    <row r="681">
+      <c r="D681" s="7"/>
+    </row>
+    <row r="682">
+      <c r="D682" s="7"/>
+    </row>
+    <row r="683">
+      <c r="D683" s="7"/>
+    </row>
+    <row r="684">
+      <c r="D684" s="7"/>
+    </row>
+    <row r="685">
+      <c r="D685" s="7"/>
+    </row>
+    <row r="686">
+      <c r="D686" s="7"/>
+    </row>
+    <row r="687">
+      <c r="D687" s="7"/>
+    </row>
+    <row r="688">
+      <c r="D688" s="7"/>
+    </row>
+    <row r="689">
+      <c r="D689" s="7"/>
+    </row>
+    <row r="690">
+      <c r="D690" s="7"/>
+    </row>
+    <row r="691">
+      <c r="D691" s="7"/>
+    </row>
+    <row r="692">
+      <c r="D692" s="7"/>
+    </row>
+    <row r="693">
+      <c r="D693" s="7"/>
+    </row>
+    <row r="694">
+      <c r="D694" s="7"/>
+    </row>
+    <row r="695">
+      <c r="D695" s="7"/>
+    </row>
+    <row r="696">
+      <c r="D696" s="7"/>
+    </row>
+    <row r="697">
+      <c r="D697" s="7"/>
+    </row>
+    <row r="698">
+      <c r="D698" s="7"/>
+    </row>
+    <row r="699">
+      <c r="D699" s="7"/>
+    </row>
+    <row r="700">
+      <c r="D700" s="7"/>
+    </row>
+    <row r="701">
+      <c r="D701" s="7"/>
+    </row>
+    <row r="702">
+      <c r="D702" s="7"/>
+    </row>
+    <row r="703">
+      <c r="D703" s="7"/>
+    </row>
+    <row r="704">
+      <c r="D704" s="7"/>
+    </row>
+    <row r="705">
+      <c r="D705" s="7"/>
+    </row>
+    <row r="706">
+      <c r="D706" s="7"/>
+    </row>
+    <row r="707">
+      <c r="D707" s="7"/>
+    </row>
+    <row r="708">
+      <c r="D708" s="7"/>
+    </row>
+    <row r="709">
+      <c r="D709" s="7"/>
+    </row>
+    <row r="710">
+      <c r="D710" s="7"/>
+    </row>
+    <row r="711">
+      <c r="D711" s="7"/>
+    </row>
+    <row r="712">
+      <c r="D712" s="7"/>
+    </row>
+    <row r="713">
+      <c r="D713" s="7"/>
+    </row>
+    <row r="714">
+      <c r="D714" s="7"/>
+    </row>
+    <row r="715">
+      <c r="D715" s="7"/>
+    </row>
+    <row r="716">
+      <c r="D716" s="7"/>
+    </row>
+    <row r="717">
+      <c r="D717" s="7"/>
+    </row>
+    <row r="718">
+      <c r="D718" s="7"/>
+    </row>
+    <row r="719">
+      <c r="D719" s="7"/>
+    </row>
+    <row r="720">
+      <c r="D720" s="7"/>
+    </row>
+    <row r="721">
+      <c r="D721" s="7"/>
+    </row>
+    <row r="722">
+      <c r="D722" s="7"/>
+    </row>
+    <row r="723">
+      <c r="D723" s="7"/>
+    </row>
+    <row r="724">
+      <c r="D724" s="7"/>
+    </row>
+    <row r="725">
+      <c r="D725" s="7"/>
+    </row>
+    <row r="726">
+      <c r="D726" s="7"/>
+    </row>
+    <row r="727">
+      <c r="D727" s="7"/>
+    </row>
+    <row r="728">
+      <c r="D728" s="7"/>
+    </row>
+    <row r="729">
+      <c r="D729" s="7"/>
+    </row>
+    <row r="730">
+      <c r="D730" s="7"/>
+    </row>
+    <row r="731">
+      <c r="D731" s="7"/>
+    </row>
+    <row r="732">
+      <c r="D732" s="7"/>
+    </row>
+    <row r="733">
+      <c r="D733" s="7"/>
+    </row>
+    <row r="734">
+      <c r="D734" s="7"/>
+    </row>
+    <row r="735">
+      <c r="D735" s="7"/>
+    </row>
+    <row r="736">
+      <c r="D736" s="7"/>
+    </row>
+    <row r="737">
+      <c r="D737" s="7"/>
+    </row>
+    <row r="738">
+      <c r="D738" s="7"/>
+    </row>
+    <row r="739">
+      <c r="D739" s="7"/>
+    </row>
+    <row r="740">
+      <c r="D740" s="7"/>
+    </row>
+    <row r="741">
+      <c r="D741" s="7"/>
+    </row>
+    <row r="742">
+      <c r="D742" s="7"/>
+    </row>
+    <row r="743">
+      <c r="D743" s="7"/>
+    </row>
+    <row r="744">
+      <c r="D744" s="7"/>
+    </row>
+    <row r="745">
+      <c r="D745" s="7"/>
+    </row>
+    <row r="746">
+      <c r="D746" s="7"/>
+    </row>
+    <row r="747">
+      <c r="D747" s="7"/>
+    </row>
+    <row r="748">
+      <c r="D748" s="7"/>
+    </row>
+    <row r="749">
+      <c r="D749" s="7"/>
+    </row>
+    <row r="750">
+      <c r="D750" s="7"/>
+    </row>
+    <row r="751">
+      <c r="D751" s="7"/>
+    </row>
+    <row r="752">
+      <c r="D752" s="7"/>
+    </row>
+    <row r="753">
+      <c r="D753" s="7"/>
+    </row>
+    <row r="754">
+      <c r="D754" s="7"/>
+    </row>
+    <row r="755">
+      <c r="D755" s="7"/>
+    </row>
+    <row r="756">
+      <c r="D756" s="7"/>
+    </row>
+    <row r="757">
+      <c r="D757" s="7"/>
+    </row>
+    <row r="758">
+      <c r="D758" s="7"/>
+    </row>
+    <row r="759">
+      <c r="D759" s="7"/>
+    </row>
+    <row r="760">
+      <c r="D760" s="7"/>
+    </row>
+    <row r="761">
+      <c r="D761" s="7"/>
+    </row>
+    <row r="762">
+      <c r="D762" s="7"/>
+    </row>
+    <row r="763">
+      <c r="D763" s="7"/>
+    </row>
+    <row r="764">
+      <c r="D764" s="7"/>
+    </row>
+    <row r="765">
+      <c r="D765" s="7"/>
+    </row>
+    <row r="766">
+      <c r="D766" s="7"/>
+    </row>
+    <row r="767">
+      <c r="D767" s="7"/>
+    </row>
+    <row r="768">
+      <c r="D768" s="7"/>
+    </row>
+    <row r="769">
+      <c r="D769" s="7"/>
+    </row>
+    <row r="770">
+      <c r="D770" s="7"/>
+    </row>
+    <row r="771">
+      <c r="D771" s="7"/>
+    </row>
+    <row r="772">
+      <c r="D772" s="7"/>
+    </row>
+    <row r="773">
+      <c r="D773" s="7"/>
+    </row>
+    <row r="774">
+      <c r="D774" s="7"/>
+    </row>
+    <row r="775">
+      <c r="D775" s="7"/>
+    </row>
+    <row r="776">
+      <c r="D776" s="7"/>
+    </row>
+    <row r="777">
+      <c r="D777" s="7"/>
+    </row>
+    <row r="778">
+      <c r="D778" s="7"/>
+    </row>
+    <row r="779">
+      <c r="D779" s="7"/>
+    </row>
+    <row r="780">
+      <c r="D780" s="7"/>
+    </row>
+    <row r="781">
+      <c r="D781" s="7"/>
+    </row>
+    <row r="782">
+      <c r="D782" s="7"/>
+    </row>
+    <row r="783">
+      <c r="D783" s="7"/>
+    </row>
+    <row r="784">
+      <c r="D784" s="7"/>
+    </row>
+    <row r="785">
+      <c r="D785" s="7"/>
+    </row>
+    <row r="786">
+      <c r="D786" s="7"/>
+    </row>
+    <row r="787">
+      <c r="D787" s="7"/>
+    </row>
+    <row r="788">
+      <c r="D788" s="7"/>
+    </row>
+    <row r="789">
+      <c r="D789" s="7"/>
+    </row>
+    <row r="790">
+      <c r="D790" s="7"/>
+    </row>
+    <row r="791">
+      <c r="D791" s="7"/>
+    </row>
+    <row r="792">
+      <c r="D792" s="7"/>
+    </row>
+    <row r="793">
+      <c r="D793" s="7"/>
+    </row>
+    <row r="794">
+      <c r="D794" s="7"/>
+    </row>
+    <row r="795">
+      <c r="D795" s="7"/>
+    </row>
+    <row r="796">
+      <c r="D796" s="7"/>
+    </row>
+    <row r="797">
+      <c r="D797" s="7"/>
+    </row>
+    <row r="798">
+      <c r="D798" s="7"/>
+    </row>
+    <row r="799">
+      <c r="D799" s="7"/>
+    </row>
+    <row r="800">
+      <c r="D800" s="7"/>
+    </row>
+    <row r="801">
+      <c r="D801" s="7"/>
+    </row>
+    <row r="802">
+      <c r="D802" s="7"/>
+    </row>
+    <row r="803">
+      <c r="D803" s="7"/>
+    </row>
+    <row r="804">
+      <c r="D804" s="7"/>
+    </row>
+    <row r="805">
+      <c r="D805" s="7"/>
+    </row>
+    <row r="806">
+      <c r="D806" s="7"/>
+    </row>
+    <row r="807">
+      <c r="D807" s="7"/>
+    </row>
+    <row r="808">
+      <c r="D808" s="7"/>
+    </row>
+    <row r="809">
+      <c r="D809" s="7"/>
+    </row>
+    <row r="810">
+      <c r="D810" s="7"/>
+    </row>
+    <row r="811">
+      <c r="D811" s="7"/>
+    </row>
+    <row r="812">
+      <c r="D812" s="7"/>
+    </row>
+    <row r="813">
+      <c r="D813" s="7"/>
+    </row>
+    <row r="814">
+      <c r="D814" s="7"/>
+    </row>
+    <row r="815">
+      <c r="D815" s="7"/>
+    </row>
+    <row r="816">
+      <c r="D816" s="7"/>
+    </row>
+    <row r="817">
+      <c r="D817" s="7"/>
+    </row>
+    <row r="818">
+      <c r="D818" s="7"/>
+    </row>
+    <row r="819">
+      <c r="D819" s="7"/>
+    </row>
+    <row r="820">
+      <c r="D820" s="7"/>
+    </row>
+    <row r="821">
+      <c r="D821" s="7"/>
+    </row>
+    <row r="822">
+      <c r="D822" s="7"/>
+    </row>
+    <row r="823">
+      <c r="D823" s="7"/>
+    </row>
+    <row r="824">
+      <c r="D824" s="7"/>
+    </row>
+    <row r="825">
+      <c r="D825" s="7"/>
+    </row>
+    <row r="826">
+      <c r="D826" s="7"/>
+    </row>
+    <row r="827">
+      <c r="D827" s="7"/>
+    </row>
+    <row r="828">
+      <c r="D828" s="7"/>
+    </row>
+    <row r="829">
+      <c r="D829" s="7"/>
+    </row>
+    <row r="830">
+      <c r="D830" s="7"/>
+    </row>
+    <row r="831">
+      <c r="D831" s="7"/>
+    </row>
+    <row r="832">
+      <c r="D832" s="7"/>
+    </row>
+    <row r="833">
+      <c r="D833" s="7"/>
+    </row>
+    <row r="834">
+      <c r="D834" s="7"/>
+    </row>
+    <row r="835">
+      <c r="D835" s="7"/>
+    </row>
+    <row r="836">
+      <c r="D836" s="7"/>
+    </row>
+    <row r="837">
+      <c r="D837" s="7"/>
+    </row>
+    <row r="838">
+      <c r="D838" s="7"/>
+    </row>
+    <row r="839">
+      <c r="D839" s="7"/>
+    </row>
+    <row r="840">
+      <c r="D840" s="7"/>
+    </row>
+    <row r="841">
+      <c r="D841" s="7"/>
+    </row>
+    <row r="842">
+      <c r="D842" s="7"/>
+    </row>
+    <row r="843">
+      <c r="D843" s="7"/>
+    </row>
+    <row r="844">
+      <c r="D844" s="7"/>
+    </row>
+    <row r="845">
+      <c r="D845" s="7"/>
+    </row>
+    <row r="846">
+      <c r="D846" s="7"/>
+    </row>
+    <row r="847">
+      <c r="D847" s="7"/>
+    </row>
+    <row r="848">
+      <c r="D848" s="7"/>
+    </row>
+    <row r="849">
+      <c r="D849" s="7"/>
+    </row>
+    <row r="850">
+      <c r="D850" s="7"/>
+    </row>
+    <row r="851">
+      <c r="D851" s="7"/>
+    </row>
+    <row r="852">
+      <c r="D852" s="7"/>
+    </row>
+    <row r="853">
+      <c r="D853" s="7"/>
+    </row>
+    <row r="854">
+      <c r="D854" s="7"/>
+    </row>
+    <row r="855">
+      <c r="D855" s="7"/>
+    </row>
+    <row r="856">
+      <c r="D856" s="7"/>
+    </row>
+    <row r="857">
+      <c r="D857" s="7"/>
+    </row>
+    <row r="858">
+      <c r="D858" s="7"/>
+    </row>
+    <row r="859">
+      <c r="D859" s="7"/>
+    </row>
+    <row r="860">
+      <c r="D860" s="7"/>
+    </row>
+    <row r="861">
+      <c r="D861" s="7"/>
+    </row>
+    <row r="862">
+      <c r="D862" s="7"/>
+    </row>
+    <row r="863">
+      <c r="D863" s="7"/>
+    </row>
+    <row r="864">
+      <c r="D864" s="7"/>
+    </row>
+    <row r="865">
+      <c r="D865" s="7"/>
+    </row>
+    <row r="866">
+      <c r="D866" s="7"/>
+    </row>
+    <row r="867">
+      <c r="D867" s="7"/>
+    </row>
+    <row r="868">
+      <c r="D868" s="7"/>
+    </row>
+    <row r="869">
+      <c r="D869" s="7"/>
+    </row>
+    <row r="870">
+      <c r="D870" s="7"/>
+    </row>
+    <row r="871">
+      <c r="D871" s="7"/>
+    </row>
+    <row r="872">
+      <c r="D872" s="7"/>
+    </row>
+    <row r="873">
+      <c r="D873" s="7"/>
+    </row>
+    <row r="874">
+      <c r="D874" s="7"/>
+    </row>
+    <row r="875">
+      <c r="D875" s="7"/>
+    </row>
+    <row r="876">
+      <c r="D876" s="7"/>
+    </row>
+    <row r="877">
+      <c r="D877" s="7"/>
+    </row>
+    <row r="878">
+      <c r="D878" s="7"/>
+    </row>
+    <row r="879">
+      <c r="D879" s="7"/>
+    </row>
+    <row r="880">
+      <c r="D880" s="7"/>
+    </row>
+    <row r="881">
+      <c r="D881" s="7"/>
+    </row>
+    <row r="882">
+      <c r="D882" s="7"/>
+    </row>
+    <row r="883">
+      <c r="D883" s="7"/>
+    </row>
+    <row r="884">
+      <c r="D884" s="7"/>
+    </row>
+    <row r="885">
+      <c r="D885" s="7"/>
+    </row>
+    <row r="886">
+      <c r="D886" s="7"/>
+    </row>
+    <row r="887">
+      <c r="D887" s="7"/>
+    </row>
+    <row r="888">
+      <c r="D888" s="7"/>
+    </row>
+    <row r="889">
+      <c r="D889" s="7"/>
+    </row>
+    <row r="890">
+      <c r="D890" s="7"/>
+    </row>
+    <row r="891">
+      <c r="D891" s="7"/>
+    </row>
+    <row r="892">
+      <c r="D892" s="7"/>
+    </row>
+    <row r="893">
+      <c r="D893" s="7"/>
+    </row>
+    <row r="894">
+      <c r="D894" s="7"/>
+    </row>
+    <row r="895">
+      <c r="D895" s="7"/>
+    </row>
+    <row r="896">
+      <c r="D896" s="7"/>
+    </row>
+    <row r="897">
+      <c r="D897" s="7"/>
+    </row>
+    <row r="898">
+      <c r="D898" s="7"/>
+    </row>
+    <row r="899">
+      <c r="D899" s="7"/>
+    </row>
+    <row r="900">
+      <c r="D900" s="7"/>
+    </row>
+    <row r="901">
+      <c r="D901" s="7"/>
+    </row>
+    <row r="902">
+      <c r="D902" s="7"/>
+    </row>
+    <row r="903">
+      <c r="D903" s="7"/>
+    </row>
+    <row r="904">
+      <c r="D904" s="7"/>
+    </row>
+    <row r="905">
+      <c r="D905" s="7"/>
+    </row>
+    <row r="906">
+      <c r="D906" s="7"/>
+    </row>
+    <row r="907">
+      <c r="D907" s="7"/>
+    </row>
+    <row r="908">
+      <c r="D908" s="7"/>
+    </row>
+    <row r="909">
+      <c r="D909" s="7"/>
+    </row>
+    <row r="910">
+      <c r="D910" s="7"/>
+    </row>
+    <row r="911">
+      <c r="D911" s="7"/>
+    </row>
+    <row r="912">
+      <c r="D912" s="7"/>
+    </row>
+    <row r="913">
+      <c r="D913" s="7"/>
+    </row>
+    <row r="914">
+      <c r="D914" s="7"/>
+    </row>
+    <row r="915">
+      <c r="D915" s="7"/>
+    </row>
+    <row r="916">
+      <c r="D916" s="7"/>
+    </row>
+    <row r="917">
+      <c r="D917" s="7"/>
+    </row>
+    <row r="918">
+      <c r="D918" s="7"/>
+    </row>
+    <row r="919">
+      <c r="D919" s="7"/>
+    </row>
+    <row r="920">
+      <c r="D920" s="7"/>
+    </row>
+    <row r="921">
+      <c r="D921" s="7"/>
+    </row>
+    <row r="922">
+      <c r="D922" s="7"/>
+    </row>
+    <row r="923">
+      <c r="D923" s="7"/>
+    </row>
+    <row r="924">
+      <c r="D924" s="7"/>
+    </row>
+    <row r="925">
+      <c r="D925" s="7"/>
+    </row>
+    <row r="926">
+      <c r="D926" s="7"/>
+    </row>
+    <row r="927">
+      <c r="D927" s="7"/>
+    </row>
+    <row r="928">
+      <c r="D928" s="7"/>
+    </row>
+    <row r="929">
+      <c r="D929" s="7"/>
+    </row>
+    <row r="930">
+      <c r="D930" s="7"/>
+    </row>
+    <row r="931">
+      <c r="D931" s="7"/>
+    </row>
+    <row r="932">
+      <c r="D932" s="7"/>
+    </row>
+    <row r="933">
+      <c r="D933" s="7"/>
+    </row>
+    <row r="934">
+      <c r="D934" s="7"/>
+    </row>
+    <row r="935">
+      <c r="D935" s="7"/>
+    </row>
+    <row r="936">
+      <c r="D936" s="7"/>
+    </row>
+    <row r="937">
+      <c r="D937" s="7"/>
+    </row>
+    <row r="938">
+      <c r="D938" s="7"/>
+    </row>
+    <row r="939">
+      <c r="D939" s="7"/>
+    </row>
+    <row r="940">
+      <c r="D940" s="7"/>
+    </row>
+    <row r="941">
+      <c r="D941" s="7"/>
+    </row>
+    <row r="942">
+      <c r="D942" s="7"/>
+    </row>
+    <row r="943">
+      <c r="D943" s="7"/>
+    </row>
+    <row r="944">
+      <c r="D944" s="7"/>
+    </row>
+    <row r="945">
+      <c r="D945" s="7"/>
+    </row>
+    <row r="946">
+      <c r="D946" s="7"/>
+    </row>
+    <row r="947">
+      <c r="D947" s="7"/>
+    </row>
+    <row r="948">
+      <c r="D948" s="7"/>
+    </row>
+    <row r="949">
+      <c r="D949" s="7"/>
+    </row>
+    <row r="950">
+      <c r="D950" s="7"/>
+    </row>
+    <row r="951">
+      <c r="D951" s="7"/>
+    </row>
+    <row r="952">
+      <c r="D952" s="7"/>
+    </row>
+    <row r="953">
+      <c r="D953" s="7"/>
+    </row>
+    <row r="954">
+      <c r="D954" s="7"/>
+    </row>
+    <row r="955">
+      <c r="D955" s="7"/>
+    </row>
+    <row r="956">
+      <c r="D956" s="7"/>
+    </row>
+    <row r="957">
+      <c r="D957" s="7"/>
+    </row>
+    <row r="958">
+      <c r="D958" s="7"/>
+    </row>
+    <row r="959">
+      <c r="D959" s="7"/>
+    </row>
+    <row r="960">
+      <c r="D960" s="7"/>
+    </row>
+    <row r="961">
+      <c r="D961" s="7"/>
+    </row>
+    <row r="962">
+      <c r="D962" s="7"/>
+    </row>
+    <row r="963">
+      <c r="D963" s="7"/>
+    </row>
+    <row r="964">
+      <c r="D964" s="7"/>
+    </row>
+    <row r="965">
+      <c r="D965" s="7"/>
+    </row>
+    <row r="966">
+      <c r="D966" s="7"/>
+    </row>
+    <row r="967">
+      <c r="D967" s="7"/>
+    </row>
+    <row r="968">
+      <c r="D968" s="7"/>
+    </row>
+    <row r="969">
+      <c r="D969" s="7"/>
+    </row>
+    <row r="970">
+      <c r="D970" s="7"/>
+    </row>
+    <row r="971">
+      <c r="D971" s="7"/>
+    </row>
+    <row r="972">
+      <c r="D972" s="7"/>
+    </row>
+    <row r="973">
+      <c r="D973" s="7"/>
+    </row>
+    <row r="974">
+      <c r="D974" s="7"/>
+    </row>
+    <row r="975">
+      <c r="D975" s="7"/>
+    </row>
+    <row r="976">
+      <c r="D976" s="7"/>
+    </row>
+    <row r="977">
+      <c r="D977" s="7"/>
+    </row>
+    <row r="978">
+      <c r="D978" s="7"/>
+    </row>
+    <row r="979">
+      <c r="D979" s="7"/>
+    </row>
+    <row r="980">
+      <c r="D980" s="7"/>
+    </row>
+    <row r="981">
+      <c r="D981" s="7"/>
+    </row>
+    <row r="982">
+      <c r="D982" s="7"/>
+    </row>
+    <row r="983">
+      <c r="D983" s="7"/>
+    </row>
+    <row r="984">
+      <c r="D984" s="7"/>
+    </row>
+    <row r="985">
+      <c r="D985" s="7"/>
+    </row>
+    <row r="986">
+      <c r="D986" s="7"/>
+    </row>
+    <row r="987">
+      <c r="D987" s="7"/>
+    </row>
+    <row r="988">
+      <c r="D988" s="7"/>
+    </row>
+    <row r="989">
+      <c r="D989" s="7"/>
+    </row>
+    <row r="990">
+      <c r="D990" s="7"/>
+    </row>
+    <row r="991">
+      <c r="D991" s="7"/>
+    </row>
+    <row r="992">
+      <c r="D992" s="7"/>
+    </row>
+    <row r="993">
+      <c r="D993" s="7"/>
+    </row>
+    <row r="994">
+      <c r="D994" s="7"/>
+    </row>
+    <row r="995">
+      <c r="D995" s="7"/>
+    </row>
+    <row r="996">
+      <c r="D996" s="7"/>
+    </row>
+    <row r="997">
+      <c r="D997" s="7"/>
+    </row>
+    <row r="998">
+      <c r="D998" s="7"/>
+    </row>
+    <row r="999">
+      <c r="D999" s="7"/>
+    </row>
+    <row r="1000">
+      <c r="D1000" s="7"/>
+    </row>
+    <row r="1001">
+      <c r="D1001" s="7"/>
+    </row>
+    <row r="1002">
+      <c r="D1002" s="7"/>
+    </row>
+    <row r="1003">
+      <c r="D1003" s="7"/>
+    </row>
+    <row r="1004">
+      <c r="D1004" s="7"/>
+    </row>
+    <row r="1005">
+      <c r="D1005" s="7"/>
+    </row>
+    <row r="1006">
+      <c r="D1006" s="7"/>
+    </row>
+    <row r="1007">
+      <c r="D1007" s="7"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -3668,6 +6730,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="4" max="4" width="28.86"/>
     <col customWidth="1" min="6" max="6" width="18.86"/>
   </cols>
   <sheetData>
@@ -3676,22 +6739,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -3719,16 +6782,16 @@
         <v>101.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>53</v>
+      <c r="D2" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E2" s="3">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="F2" s="3">
         <v>0.0</v>
@@ -3742,16 +6805,16 @@
         <v>102.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>54</v>
+      <c r="D3" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="E3" s="3">
-        <v>75.0</v>
+        <v>60.0</v>
       </c>
       <c r="F3" s="3">
         <v>0.0</v>
@@ -3765,16 +6828,16 @@
         <v>103.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C4" s="3">
         <v>3.0</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>55</v>
+      <c r="D4" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="E4" s="3">
-        <v>100.0</v>
+        <v>90.0</v>
       </c>
       <c r="F4" s="3">
         <v>0.0</v>
@@ -3788,16 +6851,16 @@
         <v>201.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C5" s="3">
         <v>1.0</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>57</v>
+      <c r="D5" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="E5" s="3">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="F5" s="3">
         <v>1.0</v>
@@ -3811,16 +6874,16 @@
         <v>202.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C6" s="3">
         <v>2.0</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>58</v>
+      <c r="D6" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="E6" s="3">
-        <v>75.0</v>
+        <v>60.0</v>
       </c>
       <c r="F6" s="3">
         <v>2.0</v>
@@ -3834,16 +6897,16 @@
         <v>203.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3">
         <v>3.0</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>59</v>
+      <c r="D7" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="E7" s="3">
-        <v>100.0</v>
+        <v>90.0</v>
       </c>
       <c r="F7" s="3">
         <v>3.0</v>
@@ -3880,7 +6943,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3911,7 +6974,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C2" s="3">
         <v>1524.0</v>
@@ -3922,7 +6985,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3">
         <v>2048.0</v>
@@ -3933,7 +6996,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Final GameData for Demo
</commit_message>
<xml_diff>
--- a/TapBand_SRC/Assets/Data/GameData.xlsx
+++ b/TapBand_SRC/Assets/Data/GameData.xlsx
@@ -75,34 +75,60 @@
     <t>FanReward</t>
   </si>
   <si>
-    <t>Falunap 1</t>
-  </si>
-  <si>
-    <t>Falunap 2</t>
-  </si>
-  <si>
-    <t>Falunap 3</t>
-  </si>
-  <si>
-    <t>Falunap 4</t>
-  </si>
-  <si>
-    <t>Falunap 5</t>
-  </si>
-  <si>
-    <t>Falunap 6</t>
-  </si>
-  <si>
-    <t>Falunap 7</t>
-  </si>
-  <si>
-    <t>Falunap 8</t>
-  </si>
-  <si>
-    <t>Falunap 9</t>
-  </si>
-  <si>
-    <t>Falunap 10</t>
+    <t>Kazincbarcikai Szabadidős Napok</t>
+  </si>
+  <si>
+    <t>Kiskunhalasi Burgonya Napok</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>SZ</t>
+    </r>
+    <r>
+      <t xml:space="preserve">abadszállási </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <t xml:space="preserve">matőr </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <t>ockfesztivál</t>
+    </r>
+  </si>
+  <si>
+    <t>Hegyalja Fesztivál</t>
+  </si>
+  <si>
+    <t>Punk Karácsony</t>
+  </si>
+  <si>
+    <t>Rockmaraton</t>
+  </si>
+  <si>
+    <t>Panksapka</t>
+  </si>
+  <si>
+    <t>Punk-Rock-Maraton</t>
+  </si>
+  <si>
+    <t>Szülinapi Koncert</t>
+  </si>
+  <si>
+    <t>Sziget Nagyszínpad</t>
   </si>
   <si>
     <t>Level</t>
@@ -2023,7 +2049,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="33.14"/>
+    <col customWidth="1" min="2" max="2" width="40.29"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>